<commit_message>
sauvegarde avant inner improvement
</commit_message>
<xml_diff>
--- a/results_1000.xlsx
+++ b/results_1000.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -37,37 +37,49 @@
     <t xml:space="preserve">StrengthenedBenders</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.5609378842872186e6, 1.5857799334898866e6, 1.682277141718253e6, 1.6901899738588037e6, 1.6916157109224645e6, 1.7107430661133826e6, 1.7182220874108502e6, 1.7183193647618503e6, 1.7265809710763306e6, 1.73447221686961e6, 1.736860327961204e6, 1.737255289681328e6, 1.751934926535737e6, 1.762445487338516e6, 1.7659861065293972e6, 1.766154494287779e6, 1.7685964160073749e6, 1.7757503718740118e6, 1.7762684878940138e6, 1.7775079784245468e6, 1.7807849567952172e6, 1.7814546216874935e6, 1.785100087642635e6, 1.7863196896530874e6, 1.7867300555616673e6, 1.7869962452984191e6, 1.789484400798983e6, 1.7901137072226757e6, 1.7915430661572462e6, 1.793378666680423e6, 1.7943843018162018e6, 1.7968278491108306e6, 1.7984042856918033e6, 1.7988147678387216e6, 1.7990072186429e6, 1.7995864417543146e6, 1.800618314739973e6, 1.8009760880957479e6, 1.8015843017548495e6, 1.8032525702820518e6, 1.8040862434312701e6, 1.8041997051223067e6, 1.8052496254022403e6, 1.8057442928305848e6, 1.8058005973866044e6, 1.8057228354408531e6, 1.806029533571109e6, 1.8059668903032402e6, 1.8059902433107307e6, 1.8060020749006707e6, 1.8060326407913312e6, 1.8062489836717986e6, 1.8062489836717988e6, 1.8073268777446104e6, 1.8074241550956105e6, 1.8077763125716103e6, 1.8077763125716103e6, 1.8079914155949587e6, 1.808602518937042e6, 1.808960904631334e6, 1.809004427395568e6, 1.8093252614391192e6, 1.8093252614391192e6, 1.8094746329249248e6, 1.8094746329249248e6, 1.8094746329249248e6, 1.809677418915119e6, 1.8100900100298051e6, 1.8101378380234772e6, 1.8101378380234772e6, 1.8101753846188616e6, 1.8104916778490236e6, 1.8112114463128773e6, 1.8116743184008517e6, 1.8116904859104487e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.8117772543021333e6, 1.811937888904955e6, 1.8123550145821134e6, 1.8123550145821134e6, 1.8123550145821134e6, 1.8126834406058579e6, 1.81283164981653e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6, 1.8128275660676216e6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941566e6, 1.875697467118622e6, 1.9433515143053252e6, 1.900876647278245e6, 1.879706576374096e6, 1.882075134186818e6, 1.8780482855865867e6, 1.9257570987146234e6, 1.9482246375682626e6, 1.921039746986001e6, 1.867362515617558e6, 1.8768901849509587e6, 1.8682666465961633e6, 1.8585447696121025e6, 1.8649251850748018e6, 1.838901094262182e6, 1.866879703441846e6, 1.8649277950126866e6, 1.8824690011439323e6, 1.838288791348785e6, 1.9110344759239203e6, 1.8684422389128169e6, 1.8487678322116763e6, 1.9051973489465832e6, 1.8431570317258143e6, 1.888011074813828e6, 1.8565485403033209e6, 1.8508033592207104e6, 1.8533051364170958e6, 1.8482565918836996e6, 1.8563815768544774e6, 1.8472083770029547e6, 1.8392166201192557e6, 1.8291782552246365e6, 1.873799421177638e6, 1.8476988873140698e6, 1.8495859784767015e6, 1.8658931182629988e6, 1.850993558033638e6, 1.8828196424077356e6, 1.836453290215526e6, 1.85737223012418e6, 1.8390648652393476e6, 1.8290083437809467e6, 1.8510464485981988e6, 1.8472380611020543e6, 1.8420829764782807e6, 1.8306496337286078e6, 1.831420929634466e6, 1.8453494573943315e6, 1.8692755700940138e6, 1.8328487167597257e6, 1.8449011854493849e6, 1.841823874967031e6, 1.8755182880686007e6, 1.831799691525922e6, 1.8519439335583097e6, 1.857949720907722e6, 1.8430389632649494e6, 1.8436616318525171e6, 1.8582269383103854e6, 1.8324461045676863e6, 1.8498588020777192e6, 1.8288764791872615e6, 1.8500044175677553e6, 1.841617521069648e6, 1.8750856648411562e6, 1.8293027653895386e6, 1.831921658474445e6, 1.84796153524534e6, 1.8696909961686528e6, 1.833394856650171e6, 1.847114079808357e6, 1.8622072469137998e6, 1.8406795761828602e6, 1.8326760901136326e6, 1.86874270253992e6, 1.8321709091615973e6, 1.846822047616373e6, 1.8296104962363776e6, 1.8543108085421415e6, 1.8879056738852898e6, 1.8317775562052063e6, 1.8302312110084926e6, 1.8430122177139733e6, 1.854147403410428e6, 1.8427691383803475e6, 1.835099415984595e6, 1.8289954493413882e6, 1.8290532877497214e6, 1.829049104798055e6, 1.829049104798055e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6, 1.8290532877497214e6]</t>
+    <t xml:space="preserve">[1.5608510252227401e6, 1.5858830097298808e6, 1.6317730597142896e6, 1.6435738021926088e6, 1.6788990491572625e6, 1.6858265869598577e6, 1.7055454845723435e6, 1.712417544033086e6, 1.7344723565842912e6, 1.7379300117629888e6, 1.7417800619992663e6, 1.7495182000483545e6, 1.7501350370281108e6, 1.7657214937799731e6, 1.7659821076080026e6, 1.766536555160042e6, 1.767554505931033e6, 1.77027856531683e6, 1.7704763998957446e6, 1.7718389699389348e6, 1.7782753070610196e6, 1.7814087883855088e6, 1.7838507268196396e6, 1.7844773883997668e6, 1.7909417630321046e6, 1.791712468877549e6, 1.7922850363305276e6, 1.7925639400603087e6, 1.7932657306314365e6, 1.7947341610406868e6, 1.7951477695762387e6, 1.7956521606690325e6, 1.7964276297737884e6, 1.796604576010184e6, 1.7968100707305642e6, 1.7969573302306698e6, 1.797164298507197e6, 1.797175178155564e6, 1.7984972876418282e6, 1.7996913367070023e6, 1.8005414873016493e6, 1.801705748818277e6, 1.8019402553282678e6, 1.8022534081492373e6, 1.802896010460576e6, 1.8031883911801078e6, 1.8034724551652274e6, 1.8038249197813098e6, 1.8044014301569331e6, 1.804752264585906e6, 1.8058030435663725e6, 1.805975455828039e6, 1.8061808821474053e6, 1.8071015839711018e6, 1.8078679221996123e6, 1.8078006212729902e6, 1.8080560889224121e6, 1.8080560889224121e6, 1.8080560889224121e6, 1.8085008967574625e6, 1.8086211518241174e6, 1.808621151824119e6, 1.808621151824119e6, 1.8094625494891675e6, 1.809564593611453e6, 1.8097198071347543e6, 1.8097198071347543e6, 1.8097390426764253e6, 1.8101424154421403e6, 1.8103086739469627e6, 1.8102300950789498e6, 1.8104621873916069e6, 1.8108201556592737e6, 1.8109520710088275e6, 1.8119124944547417e6, 1.8119124944547415e6, 1.811950377054563e6, 1.812032740818645e6, 1.8120476544055631e6, 1.8121751984449942e6, 1.8122546215312849e6, 1.812436502073124e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6, 1.8124599454023289e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941566e6, 1.879156737261e6, 1.948125623111952e6, 1.8733620792041328e6, 1.9085752213467145e6, 1.8604748129145608e6, 1.912766608702802e6, 1.8933470213253887e6, 1.9005754828877025e6, 1.8907973073099747e6, 1.923985885295588e6, 1.9022128862796146e6, 1.9039505679194282e6, 1.869955997672262e6, 1.8611791302777722e6, 1.8423265405882339e6, 1.8527435435892662e6, 1.8866216823553073e6, 1.8927370789974413e6, 1.849223272696467e6, 1.853972114053279e6, 1.9311830827066158e6, 1.8693417359695768e6, 1.8516386185991347e6, 1.835999496277409e6, 1.8770962211024931e6, 1.8557477277162739e6, 1.8486491838502407e6, 1.8583585371332958e6, 1.8694947646928441e6, 1.8480042338952564e6, 1.8575907628721704e6, 1.84170953904771e6, 1.8506420702802797e6, 1.839048761706683e6, 1.8380290081487044e6, 1.890950368906054e6, 1.8651663232744809e6, 1.8623655836355404e6, 1.8555027020666145e6, 1.8677239725255144e6, 1.8668490429242274e6, 1.8342593081457678e6, 1.8773912665716435e6, 1.8385033554293306e6, 1.831349765524295e6, 1.837760995189932e6, 1.8516438771363164e6, 1.8439525754950296e6, 1.8571977384034644e6, 1.8423510696461296e6, 1.8379137929256486e6, 1.8694061545716047e6, 1.858886789631353e6, 1.8525202299563058e6, 1.8408410194500878e6, 1.8466484052850327e6, 1.8376222064407493e6, 1.8605284797251665e6, 1.846211920484505e6, 1.848767260298086e6, 1.8398354352945394e6, 1.8672753397465104e6, 1.8401451411944798e6, 1.8331237844545308e6, 1.8425914292872578e6, 1.8502469077721883e6, 1.8578149113453247e6, 1.8488249136544762e6, 1.8416108762448474e6, 1.8515674016862514e6, 1.84679924285456e6, 1.829005170116722e6, 1.8848134961515048e6, 1.8274079580800536e6, 1.896384318615136e6, 1.8654852389904473e6, 1.8330603939404006e6, 1.8367021871023711e6, 1.8493174752206395e6, 1.83139258624155e6, 1.8284263565370531e6, 1.8346986713935018e6, 1.8349994503237878e6, 1.8321789032756032e6, 1.8421104490584258e6, 1.8360443219870746e6, 1.8316359151749045e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6, 1.8317046321225709e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.660222053527832, 1.4606730937957764, 2.1649861335754395, 2.8637120723724365, 3.6106181144714355, 4.413715124130249, 5.08502197265625, 5.762301921844482, 6.590003967285156, 7.197968006134033, 8.043429136276245, 8.746619939804077, 9.726262092590332, 10.376337051391602, 11.31303095817566, 12.103142023086548, 12.888261079788208, 13.601634979248047, 14.629211902618408, 15.309128999710083, 15.911798000335693, 16.64875292778015, 17.60725212097168, 18.19980502128601, 18.95710802078247, 19.548627138137817, 20.162459135055542, 20.800298929214478, 21.344125986099243, 21.958931922912598, 22.673671007156372, 23.380325078964233, 24.184196949005127, 24.794974088668823, 25.51122212409973, 26.112236976623535, 26.693116903305054, 27.36983895301819, 27.938832998275757, 28.583099126815796, 29.248783111572266, 29.953227996826172, 30.703460931777954, 31.25296902656555, 32.02369999885559, 32.76738905906677, 33.37173891067505, 33.96755599975586, 34.64078497886658, 35.2687349319458, 35.89488410949707, 36.486730098724365, 37.08638000488281, 37.71541905403137, 38.39100098609924, 38.915157079696655, 39.482542991638184, 40.292722940444946, 40.899336099624634, 41.57335710525513, 42.10920000076294, 42.67201495170593, 43.270097970962524, 44.00451707839966, 44.74061703681946, 45.3034610748291, 45.89651799201965, 46.6158230304718, 47.21324396133423, 47.83524012565613, 48.37027907371521, 48.97882890701294, 49.63072109222412, 50.18378210067749, 51.166682958602905, 51.729867935180664, 52.49400997161865, 53.30620312690735, 53.86322808265686, 54.46147012710571, 55.0912721157074, 55.65245199203491, 56.18045711517334, 56.77630090713501, 57.35508608818054, 57.95414996147156, 58.58925008773804, 59.215243101119995, 59.76324200630188, 60.29807710647583, 60.83493995666504, 61.399852991104126, 61.934911012649536, 62.48132801055908, 63.02662897109985, 63.57571005821228, 64.12161302566528, 64.67081093788147, 65.32821393013, 65.87999510765076, 66.42747402191162, 67.15524291992188, 67.71050596237183, 68.28413701057434, 68.8388159275055, 69.42716407775879, 70.01208806037903, 70.60270094871521, 71.17354893684387, 71.76178312301636, 72.35623908042908, 72.93649506568909, 73.5556960105896, 74.13881397247314, 74.70375490188599, 75.266685962677, 75.84762406349182, 76.42108607292175, 77.0055079460144, 77.59332799911499, 78.15989995002747, 78.75280904769897, 79.33053207397461, 79.899099111557, 80.53055191040039, 81.1117639541626, 81.6897349357605, 82.28809309005737, 82.89924597740173, 83.48227000236511, 84.06740713119507, 84.68385004997253, 85.26375102996826, 85.86399698257446, 86.4368360042572, 87.02520203590393, 87.63373613357544, 88.23210310935974, 88.84999513626099, 89.46954393386841, 90.04156398773193, 90.64167594909668, 91.26554894447327, 91.85602498054504, 92.4270191192627, 93.03741812705994, 93.61510610580444, 94.23420405387878, 94.85407304763794, 95.45555901527405, 96.04957413673401, 96.6701180934906, 97.27472996711731, 97.87397503852844, 98.47851800918579, 99.06940698623657, 99.65704202651978, 100.29001903533936, 100.89197897911072, 101.48535013198853, 102.10226511955261, 102.70434808731079, 103.28981804847717, 103.88806390762329, 104.49092292785645, 105.10985803604126, 105.7104139328003, 106.30880093574524, 106.91866111755371, 107.56972098350525, 108.16593909263611, 108.76961898803711, 109.38577508926392, 109.97790503501892, 110.58733892440796, 111.2161591053009, 111.83118891716003, 112.43652009963989, 113.06335592269897, 113.67162299156189, 114.25827503204346, 114.8611569404602, 115.49617505073547, 116.08749294281006, 116.6984441280365, 117.30848813056946, 117.91081404685974, 118.54251313209534, 119.15867805480957, 119.78142499923706, 120.43838405609131, 121.0664529800415, 121.66799592971802, 122.29738807678223, 122.91152596473694, 123.52410507202148, 124.17405104637146, 124.79271602630615, 125.39951705932617, 126.04602694511414, 126.68117713928223, 127.30601191520691, 127.94815707206726, 128.600830078125, 129.23597311973572, 129.8738260269165, 130.4941930770874, 131.10617995262146, 131.7188160419464, 132.35455298423767, 132.96801209449768, 133.60227704048157, 134.219398021698, 134.86238312721252, 135.60144209861755, 136.36667704582214, 136.99641513824463, 137.63730096817017, 138.27851390838623, 138.96473693847656, 139.61987400054932, 140.2533299922943, 140.92102003097534, 141.57806205749512, 142.2063250541687, 142.8572919368744, 143.5009400844574, 144.12775897979736, 144.8058009147644, 145.47453093528748, 146.10508704185486, 146.73622107505798, 147.38335394859314, 148.0408821105957, 148.68218111991882, 149.32407212257385, 150.00979495048523, 150.68409609794617, 151.32388305664062, 152.0164749622345, 152.65308713912964, 153.30158495903015, 153.9612500667572, 154.5968279838562, 155.26060509681702, 155.91543912887573, 156.55779695510864, 157.23676896095276, 157.88705897331238, 158.54398608207703, 159.224200963974, 159.86690402030945, 160.50571703910828, 161.16191792488098, 161.83159613609314, 162.52516913414001, 163.20747709274292, 163.85607290267944, 164.52981805801392, 165.1984989643097, 165.87087607383728, 166.5262589454651, 167.20105290412903, 167.85108494758606, 168.5380461215973, 169.22041201591492, 169.8852620124817, 170.58633303642273, 171.23830199241638, 171.90669798851013, 172.57208395004272, 173.24601006507874, 173.9629189968109, 174.63806796073914, 175.31411290168762, 176.0278971195221, 176.69162607192993, 177.35213494300842, 178.03227305412292, 178.72349905967712, 179.38032913208008, 180.04675793647766, 180.72362804412842, 181.3994641304016, 182.11654901504517, 182.80127692222595, 183.51590299606323, 184.1938190460205, 184.86577701568604, 185.5616900920868, 186.24182105064392, 186.9327630996704, 187.68574905395508, 188.3588089942932, 189.03653693199158, 189.73449206352234, 190.43100905418396, 191.16368794441223, 191.9070360660553, 192.63809895515442, 193.311861038208, 194.03015613555908, 194.70807600021362, 195.46646690368652, 196.22581911087036, 197.000097990036, 197.87188005447388, 198.66788005828857, 199.3865520954132, 200.13443613052368, 200.89861702919006, 201.59730792045593, 202.3531050682068, 203.16214203834534, 203.87740206718445, 204.63383197784424, 205.36682605743408, 206.08991694450378, 206.90165400505066, 207.61200308799744, 208.32527208328247, 209.06926202774048, 209.84410905838013, 210.55714392662048, 211.38409209251404, 212.10018801689148, 212.79816102981567, 213.5121350288391, 214.21985793113708, 214.9316771030426, 215.70436811447144, 216.41872000694275, 217.22104597091675, 217.93182706832886, 218.70104002952576, 219.46147394180298, 220.1701090335846, 220.9052391052246, 221.68189001083374, 222.38701796531677, 223.15938997268677, 223.95450806617737, 224.66623091697693, 225.3994219303131, 226.11996698379517, 226.85996007919312, 227.6481111049652, 228.4136860370636, 229.1720950603485, 229.8891899585724, 230.64604306221008, 231.49374794960022, 232.21383905410767, 232.9769480228424, 233.78348994255066, 234.50379991531372, 235.24960112571716, 235.99270296096802, 236.72542190551758, 237.5542070865631, 238.2832100391388, 239.05813193321228, 239.87329697608948, 240.60281705856323, 241.38592100143433, 242.20126509666443, 242.9480049610138, 243.70167708396912, 244.51930809020996, 245.28680896759033, 246.03313398361206, 246.8671109676361, 247.6068820953369, 248.38683104515076, 249.16593503952026, 249.90763092041016, 250.70662808418274, 251.48192596435547, 252.2265260219574, 253.03836011886597, 253.78628706932068, 254.54852390289307, 255.32777309417725, 256.08930706977844, 256.84679913520813, 257.65497398376465, 258.4056029319763, 259.2077329158783, 260.02506613731384, 260.80090498924255, 261.6248641014099, 262.3943500518799, 263.19381499290466, 264.0064070224762, 264.7775959968567, 265.5631670951843, 266.3696720600128, 267.1396210193634, 267.9662880897522, 268.74016213417053, 269.50973200798035, 270.2762141227722, 271.05325508117676, 271.849858045578, 272.77446699142456, 273.6569309234619, 274.4749300479889, 275.30285692214966, 276.0896329879761, 276.90717101097107, 277.7091009616852, 278.5465979576111, 279.34619402885437, 280.12886691093445, 280.9916069507599, 281.79598593711853, 282.62961602211, 283.4729759693146, 284.2739610671997, 285.0906901359558, 285.89746713638306, 286.69302797317505, 287.5645730495453, 288.3843951225281, 289.20242190361023, 290.0593180656433, 290.8448829650879, 291.7160339355469, 292.51501512527466, 293.32779002189636, 294.22864603996277, 295.0172619819641, 295.85323190689087, 296.73363494873047, 297.5382790565491, 298.4290499687195, 299.24972891807556, 300.05928206443787, 300.95377802848816, 301.78376293182373, 302.60469794273376, 303.4829909801483, 304.3037109375, 305.1311779022217, 305.97068095207214, 306.77203607559204, 307.6155569553375, 308.45904207229614, 309.3056299686432, 310.2081639766693, 311.0780761241913, 311.9003779888153, 312.75399112701416, 313.5711441040039, 314.4027359485626, 315.25717997550964, 316.0946099758148, 316.96445202827454, 317.8367910385132, 318.68972611427307, 319.55200695991516, 320.4050259590149, 321.2450370788574, 322.0958459377289, 322.92288613319397, 323.80815601348877, 324.65173602104187, 325.49564003944397, 326.38352704048157, 327.203978061676, 328.08886790275574, 328.9423599243164, 329.80880212783813, 330.690279006958, 331.54721999168396, 332.4462580680847, 333.32987093925476, 334.1783649921417, 335.0958800315857, 335.95063304901123, 336.83467507362366, 337.80116295814514, 338.65955090522766, 339.52117109298706, 340.4469311237335, 341.2885229587555, 342.22308897972107, 343.12061405181885, 343.9964039325714, 344.9044280052185, 345.82097601890564, 346.7088270187378, 347.55125999450684, 348.70222997665405, 349.56248712539673, 350.46057295799255, 351.34648609161377, 352.22884607315063, 353.1603651046753, 354.04298400878906, 354.93348693847656, 355.8568329811096, 356.7496349811554, 357.66110610961914, 358.53655195236206, 359.4388301372528, 360.3510539531708, 361.2227599620819, 362.1354250907898, 363.04136204719543, 363.9219059944153, 364.8918550014496, 365.7923719882965, 366.711590051651, 367.60499596595764, 368.52374505996704, 369.406800031662, 370.32404494285583, 371.2478919029236, 372.1631090641022, 373.05203008651733, 373.9646759033203, 374.8470721244812, 375.7850589752197, 376.6854500770569, 377.5863289833069, 378.5342059135437, 379.4323170185089, 380.386106967926, 381.3488349914551, 382.24170207977295, 383.1981339454651, 384.1130881309509, 385.0351369380951, 385.96153497695923, 386.8703029155731, 387.8422770500183, 388.75656294822693, 389.72009801864624, 390.6332149505615, 391.5687129497528, 392.5256209373474, 393.4344000816345, 394.460303068161, 395.36470007896423, 396.26138710975647, 397.19205594062805, 398.12697410583496, 399.1041610240936, 400.0298969745636, 400.97047090530396, 401.97426295280457, 402.93380093574524, 403.8837881088257, 404.8679609298706, 405.7672290802002, 406.82994198799133, 407.78009009361267, 408.6892111301422, 409.6418969631195, 410.57036209106445, 411.56239795684814, 412.53134512901306, 413.48248195648193, 414.4861159324646, 415.4561460018158, 416.4254651069641, 417.3697581291199, 418.33272910118103, 419.3081159591675, 420.26236605644226, 421.24074697494507, 422.2518780231476, 423.26378202438354, 424.26565313339233, 425.2303419113159, 426.24081802368164, 427.2354369163513, 428.1954469680786, 429.17981910705566, 430.14924693107605, 431.15585708618164, 432.1277720928192, 433.3647840023041, 434.3846890926361, 435.4061360359192, 436.4420509338379, 437.4397830963135, 438.4146959781647, 439.44291710853577, 440.46074295043945, 441.45587491989136, 442.4681599140167, 443.45384192466736, 444.4542860984802, 445.4467399120331, 446.4719429016113, 447.5255150794983, 448.5027301311493, 449.5647749900818, 450.5735800266266, 451.6287610530853, 452.6421239376068, 453.6198980808258, 454.5984990596771, 455.6055200099945, 456.605829000473, 457.60154390335083, 458.6443290710449, 459.64450001716614, 460.6937470436096, 461.722286939621, 462.77356004714966, 463.8225610256195, 464.8244481086731, 465.8893539905548, 466.8942971229553, 467.92102909088135, 468.9315071105957, 469.9866659641266, 471.0377459526062, 472.07050490379333, 473.10327100753784, 474.1088590621948, 475.1299579143524, 476.1504969596863, 477.1466329097748, 478.1849579811096, 479.29450511932373, 480.3385090827942, 481.40866708755493, 482.415766954422, 483.4145050048828, 484.438688993454, 485.45548701286316, 486.52466893196106, 487.5450029373169, 488.5832169055939, 489.6269910335541, 490.6805670261383, 491.8036561012268, 492.81673312187195, 493.8969509601593, 494.94257402420044, 495.9607961177826, 496.98867106437683, 498.01745104789734, 499.06862807273865, 500.09278106689453, 501.14282512664795, 502.18973207473755, 503.32297110557556, 504.36974000930786, 505.41089391708374, 506.46902203559875, 507.5073709487915, 508.58499097824097, 509.64717197418213, 510.71795105934143, 511.7623040676117, 512.8616631031036, 513.9024441242218, 514.9830420017242, 516.0403521060944, 517.0714519023895, 518.3691160678864, 519.4570600986481, 520.5493149757385, 521.6489610671997, 522.7217469215393, 523.8156099319458, 524.905436038971, 525.9751679897308, 527.0782940387726, 528.1490609645844, 529.236841917038, 530.2869029045105, 531.3845450878143, 532.4442219734192, 533.5278589725494, 534.5980100631714, 535.6876730918884, 536.7666099071503, 537.841826915741, 538.9329209327698, 540.0063309669495, 541.0907399654388, 542.1739180088043, 543.2978489398956, 544.4025249481201, 545.538211107254, 546.6312201023102, 547.7415690422058, 548.832848072052, 549.9279410839081, 551.0426840782166, 552.1199181079865, 553.2611730098724, 554.3372700214386, 555.4279670715332, 556.5144710540771, 557.6107530593872, 558.7079050540924, 559.801990032196, 560.9137749671936, 562.0861139297485, 563.2091391086578, 564.3159799575806, 565.438080072403, 566.5389699935913, 567.6967959403992, 568.7905070781708, 569.939966917038, 571.0781919956207, 572.1800389289856, 573.2941210269928, 574.4475219249725, 575.5653910636902, 576.6814019680023, 577.8112299442291, 578.9285590648651, 580.0625140666962, 581.2125539779663, 582.344633102417, 583.4507160186768, 584.6004810333252, 585.7428030967712, 586.8767640590668, 588.0174899101257, 589.2127239704132, 590.322760105133, 591.7755761146545, 592.9069061279297, 594.0973041057587, 595.2451751232147, 596.4273340702057, 597.5529599189758, 598.7057340145111, 599.8367531299591, 600.9865279197693, 602.1307621002197, 603.2856719493866, 604.4156880378723, 605.533891916275, 606.677160024643, 607.8567900657654, 609.0004739761353, 610.1609649658203, 611.3176069259644, 612.5644500255585, 613.723592042923, 614.9173469543457, 616.0577840805054, 617.2289071083069, 618.3724660873413, 619.5478000640869, 620.6959290504456, 621.8735270500183, 623.0199840068817, 624.1955769062042, 625.3304331302643, 626.527813911438, 627.683562040329, 628.9109530448914, 630.1075160503387, 631.3851771354675, 632.5568079948425, 633.7669999599457, 634.9307799339294, 636.0935399532318, 637.2484710216522, 638.4751091003418, 639.642991065979, 640.9216179847717, 642.0958380699158, 643.3338599205017, 644.4883050918579, 645.6927700042725, 646.8597309589386, 648.1451830863953, 649.3182940483093, 650.5926239490509, 651.7702131271362, 653.0360910892487, 654.2710909843445, 655.4491801261902, 656.6556279659271, 657.8612740039825, 659.0878989696503, 660.3083379268646, 661.5932140350342, 662.9372370243073, 664.4359040260315, 665.7659289836884, 667.0316579341888, 668.3339641094208, 669.5423409938812, 670.8510880470276, 672.1175169944763, 673.3692390918732, 674.5917639732361, 675.860316991806, 677.0721919536591, 678.327840089798, 679.5448789596558, 680.8449459075928, 682.1361360549927, 683.3941400051117, 684.692519903183, 685.9534559249878, 687.2233729362488, 688.4735360145569, 689.7379081249237, 690.974287033081, 692.354425907135, 693.614620923996, 694.8955399990082, 696.1953899860382, 697.4312770366669, 698.7119679450989, 699.9464859962463, 701.2491960525513, 702.5082170963287, 703.8403871059418, 705.0705111026764, 706.3591110706329, 707.6033930778503, 708.950042963028, 710.1843030452728, 711.4725959300995, 712.7113509178162, 714.020201921463, 715.2727460861206, 716.5898039340973, 717.8841559886932, 719.19176197052, 720.4885151386261, 721.801185131073, 723.0658090114594, 724.3489599227905, 725.6979739665985, 727.0198500156403, 728.339574098587, 729.6329901218414, 730.9639270305634, 732.2400999069214, 733.5895280838013, 734.8893909454346, 736.2281839847565, 737.8011291027069, 739.1291670799255, 740.4787950515747, 741.7976801395416, 743.4386250972748, 744.915205001831, 746.3697900772095, 747.7901110649109, 749.111515045166, 750.5036900043488, 751.9068140983582, 753.2739419937134, 754.6675391197205, 756.0146939754486, 757.4481210708618, 758.7925670146942, 760.1608519554138, 761.579971075058, 762.9390239715576, 764.3332250118256, 765.6783480644226, 767.0750091075897, 768.4709799289703, 769.827348947525, 771.2944920063019, 772.6502149105072, 774.1111149787903, 775.4719820022583, 776.870609998703, 778.2631211280823, 779.6307249069214, 781.027398109436, 782.4071600437164, 783.8250110149384, 785.2580671310425, 786.618115901947, 788.0712540149689, 789.4540281295776, 790.8744490146637, 792.2887969017029, 793.7389419078827, 795.1373810768127, 796.487951040268, 797.9495351314545, 799.3582310676575, 800.7795419692993, 802.2103450298309, 803.5822269916534, 805.2603940963745, 806.7380919456482, 808.147696018219, 809.6037340164185, 811.0142579078674, 812.5293729305267, 813.9690051078796, 815.4071650505066, 816.8477029800415, 818.2723820209503, 819.6727249622345, 821.0857031345367, 822.5479230880737, 823.9775810241699, 825.4260659217834, 826.8378341197968, 828.3281691074371, 829.788703918457, 831.182804107666, 832.6390120983124, 834.0981829166412, 835.5092771053314, 836.9515399932861, 838.3712511062622, 839.9361510276794, 841.3643629550934, 842.8423590660095, 844.364697933197, 845.8300220966339, 847.3000979423523, 848.7528970241547, 850.1766979694366, 851.6955380439758, 853.116672039032, 854.5936889648438, 856.050950050354, 857.4862151145935, 858.9910440444946, 860.4520649909973, 861.9057359695435, 863.4247469902039, 864.9839630126953, 866.514545917511, 868.0862140655518, 869.6699070930481, 871.3337681293488, 872.862692117691, 874.38694190979, 875.9330379962921, 877.4364221096039, 878.9283890724182, 880.5146119594574, 882.0121159553528, 883.5191900730133, 885.0712530612946, 886.5492939949036, 888.1187801361084, 889.6458320617676, 891.167366027832, 892.7257950305939, 894.1975719928741, 895.7583899497986, 897.2622089385986, 898.8817420005798, 900.4163811206818, 901.9007189273834, 903.467010974884, 905.0391449928284, 906.574569940567, 908.1334669589996, 909.7141919136047, 911.2299199104309, 912.7765080928802, 914.3354649543762, 915.8404960632324, 917.3475720882416, 918.8696749210358, 920.3896129131317, 921.928838968277, 923.5103709697723, 925.0150561332703, 926.5905020236969, 928.1466119289398, 929.6640720367432, 931.1994321346283, 932.7617719173431, 934.5576400756836, 936.1221139431, 937.7673909664154, 939.303544998169, 940.8497169017792, 942.4519639015198, 944.002571105957, 945.5697951316833, 947.1545000076294, 948.8092360496521, 950.3552050590515, 951.9904029369354, 953.5966160297394, 955.2053530216217, 956.8280100822449, 958.4279079437256, 959.9661889076233]</t>
   </si>
   <si>
     <t xml:space="preserve">LagrangianBenders</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.5609378842872186e6, 1.5857799334898866e6, 1.682277141718253e6, 1.6901899738588037e6, 1.6916157109224645e6, 1.7107430661133826e6, 1.7182220874108502e6, 1.7183193647618503e6, 1.7265809710763306e6, 1.73447221686961e6, 1.736860327961204e6, 1.737255289681328e6, 1.751934926535737e6, 1.762445487338516e6, 1.7659861065293972e6, 1.766154494287779e6, 1.7685964160073749e6, 1.7757503718740118e6, 1.7762684878940138e6, 1.7775079784245468e6, 1.7807849567952172e6, 1.7814546216874935e6, 1.785100087642635e6, 1.7863196896530874e6, 1.7867300555616673e6, 1.7869962452984191e6, 1.7894842319046434e6, 1.7902055848974448e6, 1.7922591199264105e6, 1.794623205793952e6, 1.7964312488432766e6, 1.79687679267491e6, 1.7982890242709203e6, 1.7988839863172504e6, 1.7991572186936198e6, 1.7993334211442485e6, 1.7993906293655655e6, 1.8000124851453758e6, 1.8004979911495545e6, 1.8008609058607952e6, 1.801044313027061e6, 1.801585916462636e6, 1.8022875597109324e6, 1.8022875597109324e6, 1.802521487423181e6, 1.8028235115158623e6, 1.803198661842398e6, 1.8039676881612842e6, 1.804064965512284e6, 1.804417122988284e6, 1.8054632572547176e6, 1.8054632572547174e6, 1.8054760660962942e6, 1.8054760660962942e6, 1.8054760660962942e6, 1.805482689319116e6, 1.8072607653278508e6, 1.807537787893184e6, 1.8077461114195602e6, 1.8077686283736802e6, 1.8077686283736802e6, 1.8078693206353812e6, 1.8079099422159623e6, 1.8087720958643625e6, 1.8092162525976924e6, 1.8095841914676398e6, 1.8094117792059702e6, 1.8098666897741118e6, 1.8100536374571938e6, 1.8101624317805206e6, 1.8104072381527459e6, 1.810527663511952e6, 1.8104709094702518e6, 1.8106351526075033e6, 1.8104933118685323e6, 1.8106468027314383e6, 1.8107940045540347e6, 1.8109943611090002e6, 1.8112014089208224e6, 1.8112014089208224e6, 1.8112014089208224e6, 1.8112014089208224e6, 1.8112014089208224e6, 1.8112877606972293e6, 1.8115229904716532e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.8115533331885561e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.811956302622914e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8119885464661508e6, 1.8120079545727854e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.8123410945701406e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.812273527612061e6, 1.8125905941798976e6, 1.8129176570242331e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.8129176570242334e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.813231394220428e6, 1.8132617522616675e6, 1.8134581831261113e6, 1.8134581831261113e6, 1.8134581831261113e6, 1.8134581831261113e6, 1.8134581831261113e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8134677885429652e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8137611872039684e6, 1.8138532307355097e6, 1.8138532307355097e6, 1.8139335994656328e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139335994656351e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8139568520186613e6, 1.8140946252908534e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.8140946252908532e6, 1.814484011648229e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8144840116482289e6, 1.8145712598443176e6, 1.8145712598443176e6, 1.8145712598443176e6, 1.8145712598443176e6, 1.8145712598443176e6, 1.8145712598443176e6, 1.8145771117260174e6, 1.8145771117260174e6, 1.8145771117260174e6, 1.8145771117260174e6, 1.8145771117260174e6, 1.8145771117260174e6, 1.8145993192656538e6, 1.8145993192656538e6, 1.8145993192656538e6, 1.8145993192656538e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.8148957948673076e6, 1.814929429916474e6, 1.814929429916474e6, 1.8150686395300035e6, 1.8150686395300035e6, 1.8150686395300035e6, 1.8150686395300035e6, 1.8152776318050912e6, 1.8153818309213049e6, 1.8154318027032027e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8154164160263203e6, 1.8155888282879873e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.8155888282879884e6, 1.815631187419204e6, 1.8156396776987175e6, 1.81581680444739e6, 1.8156787779676106e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8156787779676167e6, 1.8158168044473904e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.81581680444739e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.8158918603065603e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.815912682461584e6, 1.8159917997770817e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.815991799777087e6, 1.8160016574312162e6, 1.8156292339801178e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160016574312162e6, 1.8160071033392479e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160071033392476e6, 1.8160822659727521e6, 1.8160822659727517e6, 1.8160822659727517e6, 1.8160822659727517e6, 1.8160822659727517e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8161322880852157e6, 1.8164572912276122e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.8162916179548632e6, 1.816376420967511e6, 1.816376420967511e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8164437258524739e6, 1.8167265053545197e6, 1.81672650535452e6, 1.81672650535452e6, 1.81672650535452e6, 1.81672650535452e6, 1.81672650535452e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8168693099276517e6, 1.8169157129739097e6, 1.8169157129739095e6, 1.8169157129739095e6, 1.8169157129739095e6, 1.8169689056555931e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.8169689056555936e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.816978017538473e6, 1.8169945539857168e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8169945539857228e6, 1.8170631110500821e6, 1.817063111050082e6, 1.817063111050082e6, 1.817063111050082e6, 1.817065294816941e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.817065294816947e6, 1.8172399495951927e6, 1.817239949595193e6, 1.817239949595193e6, 1.817239949595193e6, 1.817239949595193e6, 1.817239949595193e6, 1.817239949595193e6, 1.8174003908430461e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174003908430464e6, 1.8174027030853634e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174200979365227e6, 1.8174215969385363e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817421596938543e6, 1.817431969505927e6, 1.817431969505927e6, 1.817431969505927e6, 1.817431969505927e6, 1.817431969505927e6, 1.817431969505927e6, 1.817484967947321e6, 1.817484967947321e6, 1.817512515996993e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175125159969935e6, 1.8175468379044551e6, 1.8175468379044551e6, 1.8175468379044551e6, 1.8175468379044551e6, 1.8175468379044551e6, 1.8175468379044551e6, 1.817695697568215e6, 1.81769569756822e6, 1.81769569756822e6, 1.81769569756822e6, 1.81769569756822e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177597138722523e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8177781327593084e6, 1.8178196596433201e6, 1.8178484837794479e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.8178882043073648e6, 1.817929204207329e6, 1.817929204207329e6, 1.817929204207329e6, 1.817929204207329e6, 1.8179147909677995e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.8179147909677993e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.817932307137991e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8179551213145268e6, 1.8181410367382166e6, 1.8181410367382169e6, 1.8181410367382169e6, 1.8181410367382169e6, 1.8182502897194983e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6, 1.8182502897195034e6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941566e6, 1.875697467118622e6, 1.9433515143053252e6, 1.900876647278245e6, 1.879706576374096e6, 1.882075134186818e6, 1.8780482855865867e6, 1.9257570987146234e6, 1.9482246375682626e6, 1.921039746986001e6, 1.867362515617558e6, 1.8769082515526253e6, 1.86828471319783e6, 1.8585628362137692e6, 1.8649432516764684e6, 1.8389191608638486e6, 1.8668977700435126e6, 1.8649458616143533e6, 1.8824690011439323e6, 1.838288791348785e6, 1.9110344759239203e6, 1.8684422389128169e6, 1.8488584850656677e6, 1.9051973489465832e6, 1.8431554611731374e6, 1.8880095042611512e6, 1.8580350139486014e6, 1.8513004077809018e6, 1.8484258176234553e6, 1.8845816816528945e6, 1.8599093778135825e6, 1.8616705164202459e6, 1.8954390450564378e6, 1.8495781517267327e6, 1.8316444802464948e6, 1.8634430458147568e6, 1.8603193835413724e6, 1.843476222703433e6, 1.8319589778891087e6, 1.8600596702766914e6, 1.8406729759219328e6, 1.8592242684950337e6, 1.862925411959131e6, 1.8272624584775919e6, 1.8514612287621244e6, 1.8494518272804448e6, 1.8755235169211354e6, 1.8469554182064242e6, 1.8416624684336034e6, 1.8582179554969885e6, 1.83603794638619e6, 1.8375053874899063e6, 1.8727214379194516e6, 1.8396028323205684e6, 1.8554850488861992e6, 1.8532319495776196e6, 1.8496150721010796e6, 1.8586145491607978e6, 1.8293123746236132e6, 1.8483493014596335e6, 1.8454796990173182e6, 1.8354632972050284e6, 1.853193751422845e6, 1.8675751415063434e6, 1.8511924086766753e6, 1.8323602164507888e6, 1.8408147152949807e6, 1.8287577436096955e6, 1.8323844730220938e6, 1.8427215640560638e6, 1.8431788376633904e6, 1.8519532411026282e6, 1.8292446669017358e6, 1.8298263113522783e6, 1.8523089063029892e6, 1.8288742752941113e6, 1.8386786338242742e6, 1.8334450435082524e6, 1.8410293166026755e6, 1.829058672346445e6, 1.832598408371101e6, 1.8349100162102075e6, 1.8459870241656795e6, 1.8378697242694835e6, 1.8488358819423688e6, 1.829098643049849e6, 1.8287599018384188e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267218e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8292221556592213e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8290902017267214e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8288177402467553e6, 1.8290727588467782e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8290248002314453e6, 1.8323891038755577e6, 1.8321180806746094e6, 1.8364324272586408e6, 1.832118080674609e6, 1.832118080674609e6, 1.832118080674609e6, 1.832118080674609e6, 1.832118080674609e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290248002314449e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8290989157556116e6, 1.8292254711116112e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437108e6, 1.8292535431437113e6, 1.8292535431437113e6, 1.8292535431437113e6, 1.8292535431437113e6, 1.8291676327032784e6, 1.8291676327032784e6, 1.829167632703278e6, 1.829167632703278e6, 1.829167632703278e6, 1.8352521233932523e6, 1.8290964601597718e6, 1.8290964601597718e6, 1.8290964601597718e6, 1.8290964601597718e6, 1.8291849118731648e6, 1.8317351102516514e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8289941824401093e6, 1.8291032074500753e6, 1.8330713252844648e6, 1.8324553720861222e6, 1.8324553720861222e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8325000638487893e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8323463470761562e6, 1.8325000638487893e6, 1.832385466163156e6, 1.8324150640238225e6, 1.8324150640238225e6, 1.8324150640238225e6, 1.8324476175171523e6, 1.8325075956577356e6, 1.832654677501842e6, 1.8326721030835654e6, 1.8326721030835654e6, 1.8327715035227356e6, 1.8326395495902356e6, 1.8326395495902356e6, 1.8326395495902356e6, 1.8326395495902356e6, 1.8326395495902356e6, 1.8326395495902356e6, 1.8328369651923203e6, 1.8328595839985274e6, 1.8328595839985274e6, 1.8328595839985274e6, 1.8328921374918567e6, 1.8328921374918567e6, 1.8328937080445334e6, 1.83287566270468e6, 1.8328595839985274e6, 1.8328595839985274e6, 1.8354213039772077e6, 1.835677053474714e6, 1.8353856966909603e6, 1.8349666909005074e6, 1.835668236593118e6, 1.8408882405778277e6, 1.835097494685505e6, 1.835082367717173e6, 1.8329434358001365e6, 1.8293906002839205e6, 1.8293745215777673e6, 1.8293745215777673e6, 1.8293745215777673e6, 1.8293745215777673e6, 1.8293854001171004e6, 1.829341968084438e6, 1.8293745215777673e6, 1.829341968084438e6, 1.8341332516565432e6, 1.832963846275605e6, 1.8329312927822752e6, 1.8330304101992713e6, 1.833124488292271e6, 1.8330304101992713e6, 1.8329978567059415e6, 1.8329978567059415e6, 1.833124412061941e6, 1.8309959344567477e6, 1.8333442069689992e6, 1.8331510876893324e6, 1.8331510876893324e6, 1.8330406110394855e6, 1.8330245323333328e6, 1.8330245323333328e6, 1.8330245323333328e6, 1.8330245323333333e6, 1.8330245323333333e6, 1.8330245323333333e6, 1.8330245323333333e6, 1.8331101771766075e6, 1.8332535920507743e6, 1.8331035909624414e6, 1.8322568261056815e6, 1.8322568261056815e6, 1.8322568261056815e6, 1.8321302707496814e6, 1.8321318413023578e6, 1.8321302707496814e6, 1.8321302707496814e6, 1.8321302707496814e6, 1.8321746574779216e6, 1.8322616471250996e6, 1.8324340593867663e6, 1.8324254919301516e6, 1.8324254919301516e6, 1.8324340593867663e6, 1.8324340593867663e6, 1.8324340593867663e6, 1.8324340593867663e6, 1.8324254919301516e6, 1.8324254919301516e6, 1.837327396564073e6, 1.8321682281086196e6, 1.8320587288379727e6, 1.8322901930687919e6, 1.832261647125099e6, 1.8322001080177992e6, 1.832168228108619e6, 1.8322953053899629e6, 1.8322282546643775e6, 1.8322152983739844e6, 1.8324392035470142e6, 1.8322873823176513e6, 1.8324392035470146e6, 1.8292682202313815e6, 1.8292356667380522e6, 1.8292682202313815e6, 1.8319649079887376e6, 1.8319649079887376e6, 1.8319649079887376e6, 1.83194843320156e6, 1.8318303664742995e6, 1.8319013308289258e6, 1.8319013308289258e6, 1.8321253534030535e6, 1.8324783925060632e6, 1.8324783925060632e6, 1.8324783925060632e6, 1.8324783925060632e6, 1.8324783925060632e6, 1.832271392433456e6, 1.832271392433456e6, 1.832271392433456e6, 1.832729802645949e6, 1.8324783925060632e6, 1.8324783925060632e6, 1.8292182866588852e6, 1.8292922037733712e6, 1.8292761250672184e6, 1.8292761250672184e6, 1.829294686580925e6, 1.8293243627937625e6, 1.8293736546864624e6, 1.82929295294813e6, 1.829294523500807e6, 1.8293090316542827e6, 1.8296291232909595e6, 1.830242813913877e6, 1.8294363678222967e6, 1.8294363678222967e6, 1.836108628149559e6, 1.8294363678222967e6, 1.829466637226906e6, 1.8296208898606615e6, 1.8294606878853284e6, 1.8295652149048147e6, 1.8296208898606615e6, 1.8296208898606615e6, 1.8296208898606615e6, 1.8295508821156474e6, 1.8299704700949045e6, 1.8292342356028587e6, 1.8292342356028587e6, 1.8292342356028587e6, 1.829308320863526e6, 1.8292342356028587e6, 1.830109729248597e6, 1.829232254638545e6, 1.8293763779077248e6, 1.8292177464850687e6, 1.829232254638545e6, 1.8292161759323918e6, 1.8292161759323918e6, 1.829072761058225e6, 1.829072761058225e6, 1.829072761058225e6, 1.8291204969415294e6, 1.8291204969415294e6, 1.8291204969415294e6, 1.8291204969415294e6, 1.8290605513240828e6, 1.8290605513240828e6, 1.8290902275369198e6, 1.8290902275369198e6, 1.8372948366956536e6, 1.835056403589708e6, 1.8290659196370828e6, 1.8288768199659626e6, 1.828951386216841e6, 1.8342504981503424e6, 1.8292182035728062e6, 1.8292180224985683e6, 1.829091648216807e6, 1.8292182033535845e6, 1.8292182033535845e6, 1.8292182033535845e6, 1.8292182033535845e6, 1.8289996952111346e6, 1.8290506305732338e6, 1.828999514356111e6, 1.8288070302004453e6, 1.828944098493111e6, 1.828944098493111e6, 1.828903119602945e6, 1.828944098493111e6, 1.828944098493111e6, 1.828944098493111e6, 1.828903119602945e6, 1.828944098493111e6, 1.828944098493111e6, 1.82895020601845e6, 1.82895020601845e6, 1.8289092271282838e6, 1.8317323972276615e6, 1.8289673111251558e6, 1.828988662563489e6, 1.8289673111251553e6, 1.8289673111251558e6, 1.8294737806696917e6, 1.8289673111251558e6, 1.8289673111251558e6, 1.8289673111251558e6, 1.8289673111251558e6, 1.8289445203382808e6, 1.828944519889286e6, 1.8294859152639976e6, 1.8289601771992643e6, 1.8296200188221957e6, 1.8327454433903603e6, 1.8289737747059485e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.8289440984931116e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.828932116990445e6, 1.8290104254027645e6, 1.828961793203282e6, 1.828944098493111e6, 1.8291165107547778e6, 1.8291165107547778e6, 1.8291165107547778e6, 1.8291165107547778e6, 1.832540432503278e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.832716352668701e6, 1.8327395653007466e6, 1.8327395653007452e6, 1.8327395653007457e6, 1.8327395653007457e6, 1.832848306601201e6, 1.8307035665425863e6, 1.8307035665425863e6, 1.8305311542809193e6, 1.8343090233775221e6, 1.8338083835013078e6, 1.8325047878087864e6, 1.8311083728332033e6, 1.8311512508772032e6, 1.830943944085717e6, 1.830863242347385e6, 1.830422380510487e6, 1.8385688574804866e6, 1.8336403278896937e6, 1.8360043098333061e6, 1.8372110212488656e6, 1.8364665959533092e6, 1.836547297691637e6, 1.836547297691637e6, 1.8372997015548672e6, 1.8432704740771886e6, 1.8328312433541093e6, 1.8326588310924426e6, 1.8305140910338277e6, 1.8305140910338277e6, 1.8326588310924426e6, 1.8305140910338277e6, 1.830341678772161e6, 1.8312365658130206e6, 1.8306986799335422e6, 1.8312024231107153e6, 1.8312024231107172e6, 1.833347163169332e6, 1.833347163169332e6, 1.832431845422753e6, 1.8325125471610783e6, 1.8303678071024637e6, 1.8303678071024637e6, 1.8303678071024637e6, 1.8303678071024637e6, 1.8309713831551569e6, 1.8309713831551569e6, 1.8309713831551569e6, 1.8309713831551569e6, 1.8353793375344402e6, 1.8342746492606862e6, 1.8341426953281867e6, 1.8307075055536567e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829429894416448e6, 1.829561848348948e6, 1.829561848348948e6, 1.829561848348948e6, 1.8289377093885883e6, 1.8289377093885883e6, 1.8289377093885883e6, 1.8289377093885883e6, 1.8297928883045085e6, 1.8297928883045085e6, 1.8297928883045085e6, 1.8297928883045067e6, 1.8297928883045085e6, 1.8297928883045085e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.829144769373278e6, 1.829144769373278e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.8302425456342155e6, 1.8291447693732784e6, 1.8291447693732784e6, 1.8337037040756762e6, 1.8291906262789445e6, 1.8292593432266114e6, 1.8293928676865695e6, 1.8293928676865695e6, 1.8293928676865695e6, 1.8293928676865695e6, 1.8293928676865695e6, 1.8293928676865695e6, 1.828960375608945e6, 1.8290182140172783e6, 1.8290182140172783e6, 1.828753315624255e6, 1.828753315624255e6, 1.828753315624255e6, 1.8288111540325887e6, 1.828753315624255e6, 1.8288111540325887e6, 1.828753315624255e6, 1.8288111540325887e6, 1.828753315624255e6, 1.8288111540325887e6, 1.828753315624255e6, 1.8614308628793156e6, 1.8328198640552906e6, 1.8325293754203527e6, 1.8347385858773047e6, 1.829186529566134e6, 1.8293277093962312e6, 1.8293277093962312e6, 1.8293277093962312e6, 1.8293277093962312e6, 1.829133853281978e6, 1.8292179287763112e6, 1.8292179287763112e6, 1.8413546485465774e6, 1.8357726213806826e6, 1.8322646605444057e6, 1.832391215900402e6, 1.8322068221360692e6, 1.8320374022118612e6, 1.8350076416868274e6, 1.8296606991083254e6, 1.8296951632677377e6, 1.8295040177728934e6, 1.8295040177728934e6, 1.8295040177728934e6, 1.8295040177728934e6, 1.8295040177728934e6, 1.8295040177728934e6, 1.8291470166115104e6, 1.832126501780115e6, 1.8319267737330608e6, 1.8320587276655608e6, 1.8629305559201469e6, 1.8321714209933472e6, 1.8321135825850153e6, 1.8320950582309486e6, 1.8321027040456808e6, 1.832360007249697e6, 1.8281758203006573e6, 1.8295232482499299e6, 1.828183466115389e6, 1.828183466115389e6, 1.828183466115389e6, 1.8321854124928243e6, 1.8322991349632055e6, 1.8321554681315143e6, 1.836985182005473e6, 1.829191312863987e6, 1.829191312863987e6, 1.829191312863987e6, 1.829191312863987e6, 1.829191312863987e6, 1.8291836670492548e6, 1.8281179818923254e6, 1.8283100214714282e6, 1.8283678598797638e6, 1.8294417886601798e6, 1.8294417886601798e6, 1.8294417886601812e6, 1.831485826848857e6, 1.831359271492863e6, 1.8289453552033207e6, 1.8289453552033207e6, 1.8289453552033207e6, 1.8289453552033207e6, 1.8289453552033207e6, 1.8313516256781318e6, 1.8313592714928635e6, 1.8313592714928635e6, 1.831434142463632e6, 1.8293709233304677e6, 1.8293709233304677e6, 1.8293709233304677e6, 1.8293709233304677e6, 1.8293632775157355e6, 1.8293709233304677e6, 1.8383238703313717e6, 1.84087437589391e6, 1.8307171730783079e6, 1.8307825333327986e6, 1.83268328619933e6, 1.8309207694950234e6, 1.8307544384248732e6, 1.8307544384248732e6, 1.8307544384248732e6, 1.8307544384248732e6, 1.8307544384248732e6, 1.8311760215291125e6, 1.8314760280101276e6, 1.8314760280101276e6, 1.8314760280101276e6, 1.8314220911796135e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8293632775157355e6, 1.8311760215291134e6, 1.831176021529113e6, 1.8308397028879118e6, 1.830839702887911e6, 1.830839702887911e6, 1.830839702887911e6, 1.8308397028879113e6, 1.830839702887911e6, 1.8308397028879113e6, 1.8308397028879113e6, 1.8291447693732781e6, 1.8290128154407782e6, 1.8288057554560886e6, 1.8288073562470465e6, 1.8288073562470465e6, 1.8288073562470465e6, 1.8288073562470465e6, 1.8293836485026977e6, 1.829323170410934e6, 1.828302375656657e6, 1.8287738482684218e6, 1.828302375656657e6, 1.8287738482684218e6, 1.8287738482684218e6, 1.8292313235832355e6, 1.8292313235832355e6, 1.8292313235832355e6, 1.8292313235832355e6, 1.829323170410934e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.8287738482684218e6, 1.8287738482684218e6, 1.8287738482684218e6, 1.8288057554560886e6, 1.8288057554560886e6, 1.829185227702445e6, 1.8291868284934028e6, 1.8293302433675695e6, 1.8293302433675695e6, 1.82933024336757e6, 1.829852270064503e6, 1.829852270064503e6, 1.829435216549166e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574022e6, 1.8293747384574027e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8298121990939947e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.8291093723055888e6, 1.8291093723055888e6, 1.8291093723055888e6, 1.8291093723055888e6, 1.8291093723055888e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.8285334156122175e6, 1.8285670622315505e6, 1.8285670622315505e6, 1.8285670622315505e6, 1.829758171324497e6, 1.829758171324497e6, 1.829758171324497e6, 1.829758171324497e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.8289491703302553e6, 1.828764776565922e6, 1.8289491703302553e6, 1.8289491703302553e6, 1.828764776565922e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.829519719311281e6, 1.8293747384574027e6, 1.8293747384574027e6, 1.8293747384574027e6, 1.8293747384574027e6, 1.8293747384574027e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.8299305835861638e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.828764776565922e6, 1.8286917236182555e6, 1.8286917236182555e6, 1.8286917236182555e6, 1.8286917236182555e6, 1.8317279659774397e6, 1.831727965977436e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8286917236182555e6, 1.8288761173825888e6, 1.831727965977436e6, 1.8286917236182555e6, 1.8288761173825888e6, 1.8286917236182555e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8286917236182555e6, 1.8286917236182555e6, 1.8286110218799221e6, 1.8318164513723277e6, 1.829255589628945e6, 1.8290711958646118e6, 1.829255589628945e6, 1.8290711958646118e6, 1.829255589628945e6, 1.8290711958646118e6, 1.8290711958646118e6, 1.831253174577556e6, 1.8311266192215737e6, 1.8311266192215728e6, 1.8311266192215732e6, 1.8310012366102398e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.8290485296442555e6, 1.829201016220922e6, 1.8290286039592554e6, 1.8290286039592554e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8290363193579218e6, 1.8308288243485754e6, 1.8308975412962344e6, 1.8308975412962344e6, 1.8308975412962511e6, 1.8308975412962511e6, 1.8308975412962511e6, 1.8308975412962511e6, 1.8292433793426114e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426119e6, 1.8292433793426114e6, 1.8292433793426114e6, 1.8292433793426114e6, 1.8292433793426114e6, 1.829275864153747e6, 1.8293626112912195e6, 1.8293626112912195e6, 1.8293626112912195e6, 1.8295469588324134e6, 1.8295469588324134e6, 1.8295469588324134e6, 1.8295469588324134e6, 1.8295469588324134e6, 1.829453829054372e6, 1.829453829054372e6, 1.829453829054372e6, 1.829453829054372e6, 1.829275864153747e6, 1.829275864153747e6, 1.829275864153747e6, 1.8293595239180694e6, 1.8293595239180694e6, 1.8293595239180694e6, 1.8293595239180694e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.828988102430724e6, 1.828988102430724e6, 1.828988102430724e6, 1.828988102430724e6, 1.828988102430724e6, 1.8284625776319834e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8291356256215298e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8290688041690574e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.8288761173825888e6, 1.829336572572501e6, 1.8314242442036024e6, 1.8314242442036024e6, 1.829336572572501e6, 1.8284625776319904e6, 1.829336572572501e6, 1.829336572572501e6, 1.8284625776319904e6, 1.8284625776319904e6, 1.8284625776320286e6, 1.829336572572501e6, 1.829336572572501e6, 1.8284625776320286e6, 1.8284625776320286e6, 1.8284625776320286e6, 1.8312976888476196e6, 1.8314242442036024e6, 1.8284625776320319e6, 1.8284625776320319e6, 1.8284289310126575e6, 1.8284289310126575e6, 1.829336572572501e6, 1.829336572572501e6, 1.829336572572501e6, 1.8284289310126575e6, 1.829336572572501e6, 1.828555486368657e6, 1.829336572572501e6, 1.829336572572501e6, 1.828555486368657e6, 1.828555486368657e6, 1.828555486368657e6, 1.829336572572501e6, 1.829336572572501e6, 1.829336572572501e6, 1.829336572572501e6, 1.829336572572501e6, 1.829336572572501e6, 1.82933483683465e6, 1.82933483683465e6, 1.82933483683465e6, 1.8290286039592554e6]</t>
+    <t xml:space="preserve">[293697.2477953015, 1.6172388592520626e6, 1.628965499467041e6, 1.6923028452272876e6, 1.7037323440228044e6, 1.7045001775952163e6, 1.7067400617085414e6, 1.7123268215723906e6, 1.7151671416344037e6, 1.7171427246181485e6, 1.7213029884213274e6, 1.7268822906103488e6, 1.7455328838685765e6, 1.746776289503285e6, 1.7468885466016592e6, 1.7496148584053647e6, 1.7514786909788703e6, 1.7518056721986386e6, 1.777210078360523e6, 1.777886812187834e6, 1.780962023075599e6, 1.7820841495822843e6, 1.7837873478967915e6, 1.7838445996267842e6, 1.7855777309510908e6, 1.785502596040424e6, 1.7860882805215486e6, 1.7861742232178762e6, 1.7894894783110155e6, 1.7894143434003487e6, 1.7916235916019806e6, 1.7919006141673136e6, 1.7928129820496673e6, 1.7927899811153337e6, 1.792812982049668e6, 1.7929623933770005e6, 1.7930498708099062e6, 1.7933226030051336e6, 1.7935050016500715e6, 1.7948950935165838e6, 1.7976205492931388e6, 1.7978735475313782e6, 1.7980564680320846e6, 1.8001606845269082e6, 1.800333096788575e6, 1.8015934411457307e6, 1.8015743076263852e6, 1.803068238226474e6, 1.8048265223925135e6, 1.805348594827305e6, 1.8055127325421036e6, 1.8059912037374694e6, 1.8060680928673365e6, 1.8061778273190353e6, 1.8063910347419083e6, 1.8065669809521409e6, 1.8064327823190116e6, 1.8064327823190116e6, 1.8068563314610708e6, 1.8068563314610708e6, 1.8068656702073996e6, 1.8081732399988582e6, 1.8089193353793817e6, 1.8093873566118267e6, 1.8095258042268024e6, 1.8095258042268027e6, 1.8095258042268027e6, 1.8095650989482899e6, 1.8096050034793532e6, 1.8099619613846664e6, 1.8100551828178284e6, 1.8103863493579137e6, 1.8108067033055816e6, 1.8112944608189994e6, 1.8119910013391846e6, 1.8124770717780718e6, 1.8128197866201065e6, 1.8128197866212842e6, 1.812870636920439e6, 1.8128991620719351e6, 1.8128273473673114e6, 1.8128273473673111e6, 1.8128273473673111e6, 1.8128273473673111e6, 1.8128273473673111e6, 1.8132091310424188e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8132091310434483e6, 1.8130123775067232e6, 1.813346222963132e6, 1.8133462229631317e6, 1.8133462229631317e6, 1.8135186352247987e6, 1.8135186352247985e6, 1.8135186352247985e6, 1.8135186352247985e6, 1.8136964985523713e6, 1.813696498552371e6, 1.813696498552371e6, 1.813696498552371e6, 1.8137240357869938e6, 1.8140177324332362e6, 1.814161398604809e6, 1.8144653089841416e6, 1.8142158656005377e6, 1.814875895091357e6, 1.814875895091583e6, 1.814875895091583e6, 1.815368520924533e6, 1.8155348199306892e6, 1.8155348199306892e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157076047052625e6, 1.8157296551769464e6, 1.8157296551769464e6, 1.8159020674322066e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8159020674386132e6, 1.8161054212288964e6, 1.8161054212288964e6, 1.8161054212288964e6, 1.8161054212288964e6, 1.8164952267534754e6, 1.8164952267541108e6, 1.8164952267541108e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8165330404723664e6, 1.8167199401374224e6, 1.8168833160616043e6, 1.8168833160616057e6, 1.8168833160616057e6, 1.8168833160616057e6, 1.8171070143671213e6, 1.8173028195125444e6, 1.8173028195125444e6, 1.8173028195125444e6, 1.8173028195125444e6, 1.8173028195125444e6, 1.8173028195125444e6, 1.8174250153692004e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174250153711042e6, 1.8174375776151298e6, 1.817437577614318e6, 1.817437577614318e6, 1.817437577614318e6, 1.817437577614318e6, 1.8174752317742112e6, 1.8174752317742112e6, 1.8174752317742112e6, 1.8174752317742112e6, 1.8174752317742112e6, 1.8175152974968166e6, 1.8176235935874218e6, 1.8176312340390114e6, 1.8176746414388986e6, 1.8176746414388986e6, 1.8177148478976164e6, 1.8177148478976164e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817785377072106e6, 1.817823623364156e6, 1.817823623364156e6, 1.8178374342246847e6, 1.817837434223997e6, 1.817837434223997e6, 1.817837434223997e6, 1.8178872601592832e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8178948869815439e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.8179877595677786e6, 1.817992459569392e6, 1.818047928115932e6, 1.818047928115932e6, 1.818047928115932e6, 1.818047928115932e6, 1.818047928115932e6, 1.818047928115932e6, 1.8180906379405789e6, 1.8180906379405789e6, 1.8180906379405789e6, 1.8180906379405789e6, 1.81815138722957e6, 1.81815138722957e6, 1.81815138722957e6, 1.8181682337969022e6, 1.8183264854289982e6, 1.8183661057120115e6, 1.8183661057120115e6, 1.8183661057120115e6, 1.8183661057120115e6, 1.818357931822162e6, 1.818371440604202e6, 1.8184909585329918e6, 1.8184909585329918e6, 1.8186873583722282e6, 1.8186873583722282e6, 1.8186873583722282e6, 1.8186873583722282e6, 1.8186201432487245e6, 1.8188810192832856e6, 1.8188810192832914e6, 1.8188810192832914e6, 1.8188810192832914e6, 1.8189046809081293e6, 1.818904680908117e6, 1.818904680908117e6, 1.818904680908117e6, 1.8189502054829977e6, 1.8189268713237091e6, 1.8189988567096686e6, 1.818998856710274e6, 1.818998856710274e6, 1.818998856710274e6, 1.818998856710274e6, 1.818998856710274e6, 1.818998856710274e6, 1.818998856710274e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190348891375135e6, 1.8190389728864243e6, 1.8190675899104853e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.819067589910814e6, 1.8190782200183796e6, 1.8191113232320691e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191113232353136e6, 1.8191724812446644e6, 1.819254956497375e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.8192549564973563e6, 1.819394313039131e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8193943130391743e6, 1.8174288432713712e6, 1.819413399237689e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194133992377967e6, 1.8194171187436876e6, 1.8195836932571738e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.819618324753692e6, 1.8196569427253027e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196569427314177e6, 1.8196663443646973e6, 1.8196663443681158e6, 1.8196663443681158e6, 1.8196943897700843e6, 1.8197974296637943e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.81979742966381e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198669321519043e6, 1.8198888859235249e6, 1.8199527241429517e6, 1.8191507859030336e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199527241429517e6, 1.8199871633452887e6, 1.819987163347615e6, 1.8200998714711664e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8200998714767448e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201251364046184e6, 1.8201432020665668e6, 1.8201432020665668e6, 1.8186389267710028e6, 1.820160899339262e6, 1.820160899339215e6, 1.820160899339215e6, 1.820160899339215e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202630131372937e6, 1.8202888125043893e6, 1.8203183227747418e6, 1.8203183227747418e6, 1.8203183227747418e6, 1.8203183227747418e6, 1.8203359772518394e6, 1.8203680120256918e6, 1.8203680120256918e6, 1.8203680120256918e6, 1.8203680120256918e6, 1.8203680120256918e6, 1.8203680120256918e6, 1.8203880924128473e6, 1.8203880924128473e6, 1.8203880924128473e6, 1.8203880924128473e6, 1.8203880924128473e6, 1.820406685063349e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.820411805383354e6, 1.8204268222087806e6, 1.820433482354467e6, 1.8205381421585437e6, 1.8205381421585437e6, 1.8206458370959524e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206458371033135e6, 1.8206499208448555e6, 1.820649920852222e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8206581511701806e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207182876149311e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207407732656596e6, 1.8207507179936685e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.8207507179932466e6, 1.820766764212469e6, 1.8207935919593764e6, 1.820257750639786e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8208312330599308e6, 1.8192319905734202e6, 1.8208910987155463e6, 1.8210518803600948e6, 1.8210518803600948e6, 1.8211066314725315e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.82110663147772e6, 1.818887913422246e6, 1.8212402116582072e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212402116588904e6, 1.8212442976092692e6, 1.8212442976092692e6, 1.8212442976092692e6, 1.8212442976092692e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.82125897251309e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212708116170692e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8212874044434146e6, 1.8213070069143001e6, 1.8213070069143001e6, 1.8213070069143001e6, 1.8213070069143001e6, 1.8213070069143001e6, 1.8213190081373835e6, 1.8213199504215159e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213199504215156e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213553653634582e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.8213714616850174e6, 1.821394104058853e6, 1.8214054764980802e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214054764983684e6, 1.8214067828872497e6, 1.8214067828872497e6, 1.8214067828872497e6, 1.8214576631935532e6, 1.8214679518991443e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215073818157404e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8215308583071523e6, 1.8216727744511443e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.821679794077407e6, 1.82169553392787e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216955339278744e6, 1.8216971079111344e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6, 1.8216971079151095e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.844825859920311e6, 1.8943093921549772e6, 1.9017901776617956e6, 1.8714522519659852e6, 1.966133884715056e6, 1.9495335236515198e6, 1.9053397739491488e6, 1.9182453672338428e6, 1.8936498441896262e6, 1.8979765636238174e6, 1.8762994189526676e6, 1.8984676430817966e6, 1.879086543926933e6, 1.8724859814004498e6, 1.9009442184555402e6, 1.933099049912465e6, 1.8706580532381814e6, 1.8961418357087e6, 1.842536695155566e6, 1.9007946863739477e6, 1.86556355755318e6, 1.9194311909960324e6, 1.8773813248875558e6, 1.8571461079385749e6, 1.850954876289012e6, 1.909993656080713e6, 1.86046416297619e6, 1.8716651973655783e6, 1.8771721528856894e6, 1.8860918218678338e6, 1.8648439306401475e6, 1.89767915391595e6, 1.8722472442540852e6, 1.8373402836574689e6, 1.8637390143293268e6, 1.862999148518788e6, 1.8633983640666243e6, 1.8567279006121142e6, 1.863437687383647e6, 1.8432046304594611e6, 1.8628304996723647e6, 1.836442445841898e6, 1.8658529842784686e6, 1.8668894010255903e6, 1.850929826709702e6, 1.8610658782540343e6, 1.8547116271140962e6, 1.9040028231491686e6, 1.868810587341235e6, 1.9153807999052634e6, 1.85942642541517e6, 1.8367918744911486e6, 1.8633668658929784e6, 1.849137770555335e6, 1.861821161569459e6, 1.870400545946756e6, 1.8391716437745355e6, 1.847147577477133e6, 1.8691709754771702e6, 1.8318946642150264e6, 1.875694255717142e6, 1.8973970899681458e6, 1.8587255393230685e6, 1.8662375361815642e6, 1.8729149129732868e6, 1.859472904170203e6, 1.8549309510299675e6, 1.857058501147478e6, 1.8452165738326209e6, 1.859194539434609e6, 1.8855510621201824e6, 1.845823322812162e6, 1.8464884964435804e6, 1.8320074288559947e6, 1.8620290380113185e6, 1.8591569506816892e6, 1.847595347742158e6, 1.9195909085620935e6, 1.868840536733401e6, 1.8495521310302746e6, 1.835259895363738e6, 1.835130268367731e6, 1.8567717529947509e6, 1.8489626337389972e6, 1.857027088151113e6, 1.8441346218177879e6, 1.8301998661442872e6, 1.8376309524759534e6, 1.8288322957555142e6, 1.8317563804478643e6, 1.833750126041535e6, 1.8335664787897908e6, 1.8432784678174898e6, 1.8327354950934364e6, 1.8414877017589496e6, 1.85340465565649e6, 1.8334128590565992e6, 1.8580625852214186e6, 1.8355045920419847e6, 1.8292696064102042e6, 1.8292696064102042e6, 1.8339578738800276e6, 1.834385720026554e6, 1.83416486974335e6, 1.8404951178273647e6, 1.903203829286031e6, 1.8370584827295113e6, 1.8354058237346683e6, 1.8292883406343122e6, 1.8329392933500095e6, 1.8328311560236022e6, 1.834463221749536e6, 1.843019962157164e6, 1.844239766088052e6, 1.8648088023918753e6, 1.829107353242732e6, 1.829107353242732e6, 1.8285508808060007e6, 1.8286774361620003e6, 1.8286659752203336e6, 1.8604670576026267e6, 1.848468466708141e6, 1.832560027493079e6, 1.8318310705889657e6, 1.8318310705889657e6, 1.832273402095306e6, 1.8361621654750437e6, 1.832445621423131e6, 1.8297174065814188e6, 1.8295994461214433e6, 1.8295994461214428e6, 1.8295994461214428e6, 1.832494734197539e6, 1.8326333872987751e6, 1.832587632379785e6, 1.832587632379785e6, 1.8496402247648046e6, 1.8527903569943293e6, 1.842933374821329e6, 1.8735220076948816e6, 1.8366051822518765e6, 1.833932787046665e6, 1.833138319255214e6, 1.83149858947229e6, 1.8324240381539606e6, 1.8380693019584615e6, 1.8385251505845673e6, 1.8440138929203968e6, 1.8624063739337954e6, 1.8296349561541274e6, 1.8337529912259942e6, 1.8327545346113287e6, 1.8330070737768358e6, 1.8296549091407864e6, 1.829654909140786e6, 1.8333239744006013e6, 1.8334889110078795e6, 1.8371477611836172e6, 1.8403429983234028e6, 1.837303452554303e6, 1.8344857460405566e6, 1.8348849742898268e6, 1.8348552980769898e6, 1.8486403355759794e6, 1.8350549170697175e6, 1.8343695528095865e6, 1.8368661899446808e6, 1.8395290700299349e6, 1.8367839445798364e6, 1.8369676588094682e6, 1.8367358935055041e6, 1.839821669506279e6, 1.8370226173857753e6, 1.836966505024788e6, 1.8369825837309407e6, 1.8371505239849463e6, 1.8371713304156258e6, 1.8309846860205454e6, 1.8335080332040542e6, 1.8397144956609735e6, 1.8376185685131315e6, 1.8360412574614326e6, 1.8365964409831276e6, 1.832713527407741e6, 1.8327211732224727e6, 1.8327211732224727e6, 1.8330712242288797e6, 1.829511020119087e6, 1.8296938097026825e6, 1.830174574204812e6, 1.8366952582704455e6, 1.833906155285408e6, 1.8330959084142984e6, 1.8312833230466882e6, 1.8468092093343388e6, 1.8332189270106556e6, 1.8345367902734962e6, 1.8283657693915556e6, 1.8339648928871818e6, 1.8352504670306842e6, 1.829871309011062e6, 1.829820045145395e6, 1.8299400259587283e6, 1.8293977586717054e6, 1.8386435690661187e6, 1.8317557720290201e6, 1.8334442194547562e6, 1.830416165927362e6, 1.843106716196386e6, 1.8623179427206751e6, 1.8293847637160618e6, 1.8465912515375528e6, 1.8315773366968792e6, 1.829715667021728e6, 1.8287512489384322e6, 1.8294525718041079e6, 1.8293259213668813e6, 1.8293259213668813e6, 1.8297323311271712e6, 1.834272260578221e6, 1.8345762824908362e6, 1.8755362812452705e6, 1.8304790995580081e6, 1.8293012116319009e6, 1.8512557102978306e6, 1.8339045769170814e6, 1.8291544935527218e6, 1.8667045707679668e6, 1.8288098526595745e6, 1.8288196766737548e6, 1.828988039606217e6, 1.828988039606217e6, 1.828988039606217e6, 1.828988039606217e6, 1.8289880396062273e6, 1.8290458780145606e6, 1.8290458780145606e6, 1.82904587801456e6, 1.8290458780145503e6, 1.8290458780145503e6, 1.8314219349275122e6, 1.8323973837068684e6, 1.8323973837068777e6, 1.8333178278291288e6, 1.8387003653265883e6, 1.8324019578020705e6, 1.832765223963179e6, 1.8289756322102405e6, 1.82910218756624e6, 1.8290762848459065e6, 1.82940661027187e6, 1.8287685722255504e6, 1.8287685722255504e6, 1.8287685722255504e6, 1.8289667658289915e6, 1.828966765827717e6, 1.8289667658414126e6, 1.8296668941733467e6, 1.8296668941733467e6, 1.8296668941596511e6, 1.8296958074894531e6, 1.8336129181158685e6, 1.8457492448045362e6, 1.8448299158688022e6, 1.829493349295234e6, 1.840307955813673e6, 1.8290937912922536e6, 1.8290937912922536e6, 1.8290937912922536e6, 1.8290937912922536e6, 1.829621507362521e6, 1.828921379030587e6, 1.828921379030587e6, 1.828921379030587e6, 1.8339512473769805e6, 1.8295465622167464e6, 1.8295325733433163e6, 1.8295325733433163e6, 1.8336112023770318e6, 1.832276761935421e6, 1.8323924387520875e6, 1.8325919032247488e6, 1.8325919032247493e6, 1.8294490951008543e6, 1.8294490951008548e6, 1.8294490951008543e6, 1.8291146391774432e6, 1.83009664337172e6, 1.8302261072721693e6, 1.8433147303068854e6, 1.8318203254953425e6, 1.8454854226844779e6, 1.8318180863079282e6, 1.830877076939861e6, 1.8310653269448394e6, 1.831065198544686e6, 1.8310653269448394e6, 1.8290725077412997e6, 1.8290725077412997e6, 1.8292918448762998e6, 1.8295066546719137e6, 1.8292918448762998e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295066546719137e6, 1.8295378025369665e6, 1.8295378025369665e6, 1.8315745674756377e6, 1.8294354584010562e6, 1.8293046968710886e6, 1.832519526335776e6, 1.8325873939910613e6, 1.8325873939910603e6, 1.8325873939910603e6, 1.829612208715893e6, 1.829612208715893e6, 1.829612208715893e6, 1.829612208715896e6, 1.829612208715893e6, 1.8292479664858489e6, 1.8292479664858489e6, 1.8292479664858489e6, 1.829219011845908e6, 1.8317155555702022e6, 1.8431433253826273e6, 1.8482259197915334e6, 1.8364166778451789e6, 1.8320058046952554e6, 1.831111589488845e6, 1.8309177839172601e6, 1.844663485628405e6, 1.8371521159163609e6, 1.844961898964654e6, 1.8375842847767884e6, 1.834190707010993e6, 1.8341675693531593e6, 1.833383674723867e6, 1.8321791860592898e6, 1.8351425196693589e6, 1.830889272656481e6, 1.8510236815199826e6, 1.8293200362374221e6, 1.8293887531850885e6, 1.8307484730327001e6, 1.8307484730327001e6, 1.8307484730327001e6, 1.8307484730327001e6, 1.8307484730327001e6, 1.8307484730327001e6, 1.8309773919557e6, 1.8333790218027548e6, 1.833097998017947e6, 1.833097998017947e6, 1.8332186207196473e6, 1.8332186207196473e6, 1.8332186207196473e6, 1.833399283022314e6, 1.832061807777743e6, 1.8320618077759494e6, 1.8320618077759494e6, 1.832076062342116e6, 1.8321330847272824e6, 1.8318696619054836e6, 1.831931150336495e6, 1.8321976218142945e6, 1.8311036830890335e6, 1.8338376756440687e6, 1.8311127773484008e6, 1.8311127773484008e6, 1.8310830211554754e6, 1.8311127773484008e6, 1.8311127773484008e6, 1.830555811438401e6, 1.8309727836612344e6, 1.830555811438401e6, 1.8685761992628912e6, 1.8324523207636348e6, 1.845847793260602e6, 1.8335916695379356e6, 1.8335922512763895e6, 1.8328771247252177e6, 1.8321908907205418e6, 1.8341125487245058e6, 1.8340796287910456e6, 1.8342061841470457e6, 1.8342061841470457e6, 1.8342061841470457e6, 1.8373141847812773e6, 1.8341546828677498e6, 1.8314277447475076e6, 1.8306718576744667e6, 1.8306718576744667e6, 1.8314492901518743e6, 1.8306718576744667e6, 1.83472369503006e6, 1.8312351344692518e6, 1.8320181727297378e6, 1.8321451995336565e6, 1.832159454099823e6, 1.8320504993042035e6, 1.833536023741963e6, 1.8339265948589311e6, 1.8307220502680677e6, 1.8371268818625186e6, 1.8363510012819914e6, 1.8347993338927191e6, 1.8333299263210392e6, 1.8326727077431458e6, 1.8310944781009478e6, 1.832002493136939e6, 1.8293244677205745e6, 1.8309260371984483e6, 1.8309260371984483e6, 1.8307994818424482e6, 1.8293451917779518e6, 1.8293404007215917e6, 1.8293404007215917e6, 1.8293404007215917e6, 1.8290953005041324e6, 1.829343431571924e6, 1.8293481471689132e6, 1.8293481471689132e6, 1.8290517991842388e6, 1.8291000161011212e6, 1.8291000161011212e6, 1.8291000161011207e6, 1.8294053408773632e6, 1.8302055578228764e6, 1.8292667510335434e6, 1.8292667510335438e6, 1.8292180978636032e6, 1.829487763050957e6, 1.829487763050957e6, 1.8382330278048718e6, 1.8420266244493078e6, 1.836711023352733e6, 1.8292506225378138e6, 1.8307167734770116e6, 1.830389436031068e6, 1.830262880675068e6, 1.8425712576575156e6, 1.8295692768338278e6, 1.829537180494934e6, 1.8297536705981612e6, 1.828185512322374e6, 1.8298734557407356e6, 1.836200077627458e6, 1.834701139378004e6, 1.8346324224303372e6, 1.8341816585818653e6, 1.8301333597817172e6, 1.8301333597817172e6, 1.830617128117229e6, 1.8340856264371702e6, 1.8338777212908964e6, 1.837167753166234e6, 1.848921792246334e6, 1.8314872894052716e6, 1.8356677549299772e6, 1.8295041218621659e6, 1.8360607510129835e6, 1.8297430048299169e6, 1.8295041218621659e6, 1.829311074130214e6, 1.829311074130214e6, 1.8310124479036143e6, 1.8296245925840337e6, 1.8296978893310886e6, 1.8296978893310886e6, 1.8341542112842395e6, 1.8326375321056356e6, 1.8343736344864948e6, 1.8369797567592605e6, 1.834500189842495e6, 1.834500189842495e6, 1.8577019749663e6, 1.832559736083125e6, 1.8334043128978743e6, 1.8389267724501493e6, 1.837103111444418e6, 1.8354024765205334e6, 1.8281290056610408e6, 1.8346199061351276e6, 1.8340215476182217e6, 1.8297659706513134e6, 1.8297659706513134e6, 1.8298314039167783e6, 1.8299318307764425e6, 1.8344071807408228e6, 1.8628557592511468e6, 1.8326407792426937e6, 1.8317432421807374e6, 1.8293667336380787e6, 1.8293209787190885e6, 1.8295769574758809e6, 1.8295769574758809e6, 1.830102905314088e6, 1.8297624852907553e6, 1.8297624852907553e6, 1.8297624852907553e6, 1.8297624852907553e6, 1.8293275951967554e6, 1.829121359913695e6, 1.8298421318870827e6, 1.8326335806540528e6, 1.8336826179725009e6, 1.8337327641353665e6, 1.8330860665826474e6, 1.8323968994818318e6, 1.8321237736762294e6, 1.8345103575897806e6, 1.8334358758018732e6, 1.8368506963533654e6, 1.835822511920912e6, 1.834838152570953e6, 1.831301971832548e6, 1.8477812058389706e6, 1.8613897259181885e6, 1.831893076111594e6, 1.8333466112450382e6, 1.8338122020051565e6, 1.829791119570439e6, 1.8296298250372636e6, 1.8296298250372636e6, 1.829629825037263e6, 1.8296298250372636e6, 1.834593420930329e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8295772194209096e6, 1.8332415369368314e6, 1.832542140816245e6, 1.8298981513768474e6, 1.8298981513768474e6, 1.8298981513768474e6, 1.831075414762615e6, 1.8294735241069098e6, 1.8294735241069098e6, 1.8294735241069093e6, 1.8294735241069098e6, 1.8294735241069098e6, 1.8294735241069098e6, 1.8294891287641122e6, 1.8298159605042816e6, 1.8298159605042816e6, 1.8298159605042816e6, 1.8298159605042816e6, 1.8313003745068137e6, 1.8323883048856708e6, 1.8322644594130039e6, 1.833495036909396e6, 1.8307819560582472e6, 1.8307819560582472e6, 1.8307819560582472e6, 1.831086414805235e6, 1.831086414805235e6, 1.831086414805235e6, 1.831086414805235e6, 1.831086414805235e6, 1.831086414805235e6, 1.829803537690046e6, 1.830054666569913e6, 1.830054666569912e6, 1.830054666569912e6, 1.8300315289120788e6, 1.8300315289120788e6, 1.8300315289120788e6, 1.8300315289120788e6, 1.8334381007608676e6, 1.8330147552879772e6, 1.8306248442470504e6, 1.836008736849366e6, 1.831547480692675e6, 1.8316039555142412e6, 1.8316039555142412e6, 1.8316039555142412e6, 1.8316039555142412e6, 1.8316039555142412e6, 1.8296418389490887e6, 1.8334412167878335e6, 1.8334412167878335e6, 1.8346287261734863e6, 1.8346287261734863e6, 1.829772491724576e6, 1.8299910399024778e6, 1.8299910399024778e6, 1.8299910399024778e6, 1.8301575924344778e6, 1.8304253907079205e6, 1.829794122619978e6, 1.829794122619978e6, 1.850789710247114e6, 1.8350394099234531e6, 1.8355510458191058e6, 1.8356776011751026e6, 1.8356776011751026e6, 1.8356776011751026e6, 1.8368530977605192e6, 1.8348277828448347e6, 1.840094214777286e6, 1.830588885866259e6, 1.830536911978664e6, 1.830536911978665e6, 1.8304681950309977e6, 1.8304681950309977e6, 1.8304681950309982e6, 1.8301336114087205e6, 1.830170739987036e6, 1.833790824845392e6, 1.8359722513072945e6, 1.8349566817696278e6, 1.8590826543482116e6, 1.8316308172617003e6, 1.8301411624735205e6, 1.8301411624735205e6, 1.8301833144591872e6, 1.8301833144591872e6, 1.8301833144591877e6, 1.8301026127208548e6, 1.8303260214175207e6, 1.8301026127208548e6, 1.8301145975115208e6, 1.8301145975115208e6, 1.8301145975115208e6, 1.8301145975115208e6, 1.833864942645877e6, 1.8349743768251224e6, 1.8324777617842846e6, 1.8324777617842846e6, 1.8324252916889514e6, 1.8332099207603706e6, 1.8324884984102848e6, 1.8325991009044515e6, 1.8325991009044515e6, 1.8325991009044515e6, 1.8325991009044515e6, 1.8325991009044515e6, 1.8325991009044515e6, 1.8332683854834277e6, 1.8326515709997846e6, 1.8330367495092617e6, 1.8326292337221086e6, 1.8363405961756834e6, 1.831650074695524e6, 1.8318681150791908e6, 1.8317187916431904e6, 1.8317187916431904e6, 1.8335549178721572e6, 1.833562916226833e6, 1.831527544394837e6, 1.830807003179448e6, 1.830807003179448e6, 1.830807003179448e6, 1.830807003179448e6, 1.830807003179448e6, 1.8304221953302214e6, 1.8337931106988958e6, 1.830601288240296e6, 1.8337319130448552e6, 1.8481520275970225e6, 1.8422029362029417e6, 1.8314867306350663e6, 1.8295217909709855e6, 1.8293133221315762e6, 1.8293819851468096e6, 1.8295139088158098e6, 1.8295139088158112e6, 1.8293133221315762e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295139088158098e6, 1.8295475554351432e6, 1.8303214999045006e6, 1.831735268335628e6, 1.8317406366486282e6, 1.831614081292628e6, 1.8367186054346368e6, 1.8292862039655808e6, 1.8292862039655803e6, 1.8292862039655803e6, 1.830303408412888e6, 1.828361249638534e6, 1.8303034084128889e6, 1.8328381007971622e6, 1.829748790157343e6, 1.8413435136431188e6, 1.8322484020967844e6, 1.8322375235574509e6, 1.8322375235574509e6, 1.8295260871459825e6, 1.8295260871459825e6, 1.8347601770252006e6, 1.8304069411558912e6, 1.837770154756354e6, 1.8330813775629138e6, 1.8303034084128889e6, 1.8303034084128889e6, 1.8321740296817005e6, 1.8297298159761752e6, 1.8279033340184803e6, 1.8279033340184803e6, 1.82777141034948e6, 1.8297876543845006e6, 1.8325312116048431e6, 1.829910667819565e6, 1.8298984622421523e6, 1.8298984622421523e6, 1.8298984622421523e6, 1.8298984622421523e6, 1.8298984622421523e6, 1.8395479654240778e6, 1.831194312498124e6, 1.8297347928392359e6, 1.8298667165082355e6, 1.830026918483569e6, 1.8298154868540836e6, 1.8298154868540836e6, 1.8298154868540836e6, 1.8298154868540836e6, 1.8296082297597507e6, 1.8298453782137472e6, 1.8303617493674268e6, 1.8295414821749025e6, 1.8345335778598234e6, 1.8318627008881227e6, 1.8343273886917958e6, 1.8324383823987104e6, 1.8331084838187646e6, 1.831456726158228e6, 1.8311960263505417e6, 1.8363528198415881e6, 1.8335743994972392e6, 1.833288275774292e6, 1.8320301617448453e6, 1.8387932812913072e6, 1.8318169131167082e6, 1.8397801667969485e6, 1.831748172735391e6, 1.8286989463545016e6, 1.8302066045691634e6, 1.8290155280185228e6, 1.8362684908366061e6, 1.8339726691591993e6, 1.837775528866072e6, 1.8336449878662208e6, 1.832442609430204e6, 1.8338703322965673e6, 1.8328890893947121e6, 1.8297954946616495e6, 1.8326871170310455e6, 1.8324086040721175e6, 1.8324381641741174e6, 1.8324664424804507e6, 1.832526915055712e6, 1.8302681074583756e6, 1.8326542681119775e6, 1.8323831734333106e6, 1.8323831734333106e6, 1.8323831734333106e6, 1.8323831734333106e6, 1.8399180861752064e6, 1.8370907951407477e6, 1.842725035085051e6, 1.8358964202334925e6, 1.8372509339202067e6, 1.8386342309565924e6, 1.8369697402603894e6, 1.8329335793166545e6, 1.8329335793166545e6, 1.8329335793166545e6, 1.8364052494710342e6, 1.8291937925152795e6, 1.831870330417663e6, 1.8318904742757736e6, 1.8317525232541047e6, 1.831985214826586e6, 1.8339199945761703e6, 1.828687439189791e6, 1.828847641165125e6, 1.828847641165125e6, 1.828847641165125e6, 1.828847641165125e6, 1.828847641165124e6, 1.8369322171025707e6, 1.833903646237055e6, 1.836194728678834e6, 1.8429511800292025e6, 1.8332923317562838e6, 1.8325524856609532e6, 1.832749865593773e6, 1.8325686798314934e6, 1.8323187813027233e6, 1.829804789972686e6, 1.8294045164287619e6, 1.82902743587796e6, 1.8288659305106264e6, 1.8288659305106264e6, 1.8288659305106264e6, 1.8290236433356784e6, 1.8290236433356784e6, 1.8290558509838886e6, 1.8292979561988886e6, 1.8368963622465243e6, 1.8296471490443868e6, 1.8498463599089303e6, 1.8460595851118162e6, 1.8332062736656938e6, 1.833201419971408e6, 1.8332062736656938e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8331081423047173e6, 1.8298826332852861e6, 1.8299148409334964e6, 1.8299148409334964e6, 1.8322418119240876e6, 1.8331862173823284e6, 1.8335908539764008e6, 1.8298826332852861e6, 1.8333711671760438e6, 1.8331216850559919e6, 1.8331049153565748e6, 1.8333647671066958e6, 1.828828865314199e6, 1.828828865314199e6, 1.828958132418603e6, 1.8321800778936802e6, 1.8327196608423258e6, 1.8325702498798112e6, 1.8288087214560884e6, 1.8289045424392696e6, 1.828828865314199e6, 1.8288446378509214e6, 1.8288038259869365e6, 1.8287966576659887e6, 1.8295261031592141e6, 1.8293736165825499e6, 1.8293736165825499e6, 1.8294314549908813e6, 1.8294314549908813e6, 1.8294314549908813e6, 1.8294314549908813e6, 1.8294314549908813e6, 1.8294314549908813e6, 1.82878228041627e6, 1.82878228041627e6, 1.82878228041627e6, 1.82878228041627e6, 1.831954708143154e6, 1.8308900509090193e6, 1.833822878900532e6, 1.8328595292927132e6, 1.8294849097738133e6, 1.8294849097738133e6, 1.82942707136548e6, 1.82942707136548e6, 1.8332503373540451e6, 1.8339411072987549e6, 1.8335579575600515e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8289546926779367e6, 1.8290358965119363e6, 1.8325657368319992e6, 1.8320227301126763e6, 1.8341854969918185e6, 1.829281854172603e6, 1.829281854172603e6, 1.8297775131730887e6, 1.8295425226436283e6, 1.82933956562327e6, 1.829347985603072e6, 1.82933956562327e6, 1.82933956562327e6, 1.8344347146145275e6, 1.831410421885948e6, 1.831410421885948e6, 1.8321497246354374e6, 1.8340059568105561e6, 1.838198568616439e6, 1.8321497246354374e6, 1.8321497246354374e6, 1.8321497246354374e6, 1.8329161838546565e6, 1.8318534559785698e6, 1.8318534559785698e6, 1.8318233422893917e6, 1.8318233422893917e6, 1.831650930027725e6, 1.831681043716903e6, 1.831681043716903e6, 1.8279020022714797e6, 1.8310865331642812e6, 1.8310865331642812e6, 1.8310865331642812e6, 1.8310865331642812e6, 1.8310865331642812e6, 1.8364083409890013e6, 1.8292375862848905e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8289454606405573e6, 1.8342375096047877e6, 1.8442512473328782e6, 1.8341367830976692e6, 1.832424003769521e6, 1.8335440932092008e6, 1.8337722903193615e6, 1.8352795581167222e6, 1.8279020022714797e6, 1.8279020022714797e6, 1.832348037113339e6, 1.83240778624324e6, 1.8453853503207278e6, 1.8333615533206018e6, 1.8331433247697263e6, 1.833883940671961e6, 1.8312506367174357e6, 1.8311482731504363e6, 1.8312506367174361e6, 1.8345940512818892e6, 1.8317890554631313e6, 1.83139428638557e6, 1.8318170539032335e6, 1.8315208417415696e6, 1.8321539845724644e6, 1.8289015749253302e6, 1.8286910830000888e6, 1.8368179639931454e6, 1.8290027838065156e6, 1.8290027838065156e6, 1.8290027838065156e6, 1.8290027838065156e6, 1.8290027838065156e6, 1.8290027838065156e6, 1.8288441293562201e6, 1.8290381213993628e6, 1.8336298488945335e6, 1.8336298488945335e6, 1.833629848894534e6, 1.833629848894534e6, 1.8292208656903931e6, 1.8292208656903931e6, 1.8292208656903931e6, 1.8292208656903931e6, 1.8292208656903931e6, 1.8288404315341117e6, 1.8298909789280042e6, 1.8289952185331115e6, 1.828995218533112e6, 1.8293253392149138e6, 1.8293253392149138e6, 1.8295964338935802e6, 1.8297579392609133e6, 1.8293945589992858e6, 1.8292343570239523e6, 1.8292343570239523e6, 1.8281572340160406e6, 1.8335851649017024e6, 1.8335164479540356e6, 1.8336978029976033e6, 1.8293599013820507e6, 1.8293599013820507e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.830268248988068e6, 1.8305697864365557e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.1304419040679932, 2.2519779205322266, 3.9052088260650635, 4.880275011062622, 6.211261987686157, 7.610984802246094, 9.141908884048462, 10.989498853683472, 12.794534921646118, 14.562013864517212, 15.966801881790161, 17.526376962661743, 18.872668981552124, 20.170362949371338, 21.581851959228516, 23.311482906341553, 25.2636559009552, 26.796430826187134, 27.882539987564087, 29.215848922729492, 30.52773380279541, 32.128718852996826, 33.78543400764465, 35.41761302947998, 36.851974964141846, 38.440157890319824, 40.03873300552368, 41.41039800643921, 42.977571964263916, 44.49650001525879, 46.01503300666809, 47.64111089706421, 49.21050786972046, 50.548550844192505, 52.02785301208496, 53.5560359954834, 55.14305090904236, 56.60849189758301, 58.20984983444214, 59.57855796813965, 61.06922698020935, 62.37843203544617, 63.81977200508118, 65.29291796684265, 66.78540682792664, 68.41073894500732, 70.11040592193604, 71.86107587814331, 73.72908282279968, 75.54516100883484, 77.25677394866943, 78.7514100074768, 80.57377600669861, 82.28324580192566, 83.96268796920776, 85.79294490814209, 87.40918183326721, 89.25633096694946, 91.0404589176178, 92.5957579612732, 94.59471988677979, 96.57387781143188, 98.2890830039978, 100.21821093559265, 102.12071585655212, 103.81138300895691, 105.52472400665283, 107.5261800289154, 109.32060384750366, 111.17859196662903, 113.14572095870972, 114.78496980667114, 116.53603100776672, 118.34492897987366, 120.49901986122131, 122.16442084312439, 124.042888879776, 126.31517601013184, 128.17699885368347, 130.19013500213623, 131.91591000556946, 133.5339639186859, 135.4328429698944, 137.25223302841187, 139.1902458667755, 141.0989899635315, 142.8447709083557, 144.80212783813477, 146.38801383972168, 148.0129909515381, 149.92203998565674, 151.66556096076965, 153.54812097549438, 155.27297401428223, 157.14360880851746, 159.15411496162415, 160.80618286132812, 162.868999004364, 164.66244196891785, 166.49834203720093, 168.21293783187866, 170.14176201820374, 171.79199481010437, 173.6508708000183, 175.605947971344, 177.8792769908905, 179.6730020046234, 181.60592103004456, 183.41945385932922, 185.205237865448, 187.37727785110474, 189.2711570262909, 191.49948287010193, 193.539705991745, 195.9736189842224, 198.19690990447998, 200.2057240009308, 202.50565195083618, 204.6236228942871, 206.74395489692688, 209.15604782104492, 211.4478030204773, 213.22597289085388, 214.91808986663818, 217.00921392440796, 219.10694885253906, 221.3304660320282, 223.2671139240265, 225.0686240196228, 227.00537300109863, 228.95653581619263, 231.1474769115448, 233.2027108669281, 235.1326389312744, 237.21460890769958, 239.3031530380249, 241.75047397613525, 244.07471585273743, 246.24035692214966, 248.6056900024414, 250.7906138896942, 252.83760690689087, 254.92576694488525, 256.98461985588074, 259.0710029602051, 261.3497989177704, 263.52849888801575, 265.7752888202667, 268.1936619281769, 270.15915083885193, 272.142942905426, 274.2220849990845, 276.30019998550415, 278.38006591796875, 280.5432388782501, 282.845666885376, 284.8836770057678, 287.15378403663635, 289.4913578033447, 291.60783791542053, 293.86253786087036, 296.03709387779236, 298.2619960308075, 300.68314599990845, 303.2339828014374, 305.3668968677521, 307.56198287010193, 310.0382950305939, 312.4031388759613, 314.6864058971405, 317.0591540336609, 319.2786478996277, 321.4078879356384, 323.552503824234, 325.79788398742676, 327.9366238117218, 330.2614870071411, 332.40651988983154, 334.728492975235, 337.37794494628906, 339.686970949173, 342.167062997818, 344.34070682525635, 346.45565700531006, 348.4591908454895, 350.5489308834076, 353.0408179759979, 355.2063148021698, 357.4071238040924, 359.581964969635, 361.8252890110016, 364.30077385902405, 366.58918380737305, 368.72036695480347, 371.10863494873047, 373.31299781799316, 375.50338196754456, 377.63950300216675, 380.10233783721924, 382.5246000289917, 384.8512578010559, 387.1465919017792, 389.3312849998474, 391.68190598487854, 394.2155818939209, 396.49410796165466, 398.8644669055939, 401.34327602386475, 403.82394790649414, 406.6313989162445, 409.0129280090332, 411.5595259666443, 414.1049180030823, 416.32058596611023, 418.55146193504333, 420.86619091033936, 423.3596088886261, 425.78016781806946, 427.9652359485626, 430.5564420223236, 433.1223199367523, 436.18974900245667, 438.7574670314789, 441.15950989723206, 443.6967179775238, 446.1732339859009, 448.5965328216553, 451.3727328777313, 453.6161639690399, 455.8036849498749, 458.0382878780365, 460.20355582237244, 462.55882501602173, 465.02692103385925, 467.2809188365936, 469.62015295028687, 471.8618378639221, 474.1105580329895, 476.25576400756836, 478.88803791999817, 481.3754029273987, 483.5468029975891, 485.8169958591461, 488.216295003891, 491.11657786369324, 493.6669239997864, 495.99722599983215, 498.392413854599, 500.5887768268585, 503.1462559700012, 505.4702858924866, 507.62800884246826, 509.9072198867798, 512.2084469795227, 514.5186610221863, 516.6153388023376, 518.7558748722076, 521.1454730033875, 523.4512979984283, 525.7202048301697, 528.0989990234375, 530.3977479934692, 532.8067269325256, 535.2748649120331, 537.7861618995667, 540.2530670166016, 542.8690760135651, 545.2809419631958, 547.915608882904, 550.2985129356384, 552.5865669250488, 554.8150069713593, 557.2579469680786, 559.4121129512787, 562.2121360301971, 564.7150869369507, 567.204806804657, 569.519357919693, 571.7762529850006, 574.1537978649139, 576.462975025177, 578.8721129894257, 581.1734638214111, 583.4525499343872, 585.7979040145874, 588.3860239982605, 590.8675088882446, 593.2793779373169, 595.9575529098511, 598.4080448150635, 600.6465888023376, 603.1888270378113, 605.3614029884338, 607.6479978561401, 609.9662508964539, 612.4079859256744, 614.7083308696747, 617.0236299037933, 619.1425130367279, 621.3441379070282, 623.5101838111877, 625.8127179145813, 628.3065299987793, 630.8155310153961, 633.1095700263977, 635.4439070224762, 637.8024978637695, 640.317843914032, 642.8410778045654, 645.2443978786469, 647.7236399650574, 650.4649069309235, 653.2919719219208, 655.8563168048859, 658.2267990112305, 660.7700109481812, 663.1108210086823, 665.6380100250244, 668.2655649185181, 670.7881460189819, 672.9981558322906, 675.362872838974, 677.600014925003, 680.0646369457245, 682.3631689548492, 684.6954689025879, 687.1537148952484, 689.5697050094604, 692.4454419612885, 695.4754049777985, 698.3008878231049, 700.9563210010529, 703.3602368831635, 705.819100856781, 708.436117887497, 710.8810498714447, 713.3463349342346, 716.0166249275208, 718.3483300209045, 720.7592868804932, 723.0382328033447, 725.5972249507904, 728.0673139095306, 730.5282018184662, 733.1574838161469, 735.6429669857025, 737.930979013443, 740.4301788806915, 742.8802309036255, 745.2628388404846, 747.507269859314, 749.792662858963, 752.1361320018768, 754.449798822403, 757.1514298915863, 759.5124599933624, 761.70942902565, 764.0287458896637, 766.2312698364258, 768.5380308628082, 771.0061860084534, 773.6394469738007, 775.9469788074493, 778.3461968898773, 780.616367816925, 782.9136798381805, 785.3339760303497, 787.5595939159393, 789.9208738803864, 792.4221968650818, 794.9345278739929, 797.4417128562927, 799.803505897522, 802.2149758338928, 804.42480301857, 806.8913550376892, 809.3250789642334, 811.9015758037567, 814.4212069511414, 817.3082139492035, 819.7997260093689, 822.4710638523102, 824.8436408042908, 827.2195229530334, 829.5778360366821, 831.7627580165863, 834.1667778491974, 836.5732629299164, 839.114198923111, 841.4973428249359, 843.80841588974, 846.4049088954926, 848.7995069026947, 851.447732925415, 853.8307318687439, 856.1084229946136, 858.3715770244598, 860.5904660224915, 863.2603259086609, 865.7079439163208, 867.9552898406982, 870.1833229064941, 872.3470849990845, 874.6176338195801, 877.1751129627228, 879.8203608989716, 882.219810962677, 884.8661479949951, 887.366662979126, 889.9432389736176, 892.5370059013367, 895.0411558151245, 897.6700918674469, 900.1829679012299, 902.5245590209961, 905.2242958545685, 907.5531978607178, 909.9154558181763, 912.470470905304, 914.6135578155518, 916.6989698410034, 918.8028018474579, 920.9969999790192, 923.2679979801178, 925.5219688415527, 927.740327835083, 930.0814788341522, 932.4537208080292, 934.6039910316467, 936.9776659011841, 939.2609369754791, 941.6084818840027, 944.006954908371, 946.2083518505096, 948.6198279857635, 951.0634369850159, 953.508083820343, 956.0189509391785, 958.5129828453064, 961.0525858402252, 963.2704880237579, 965.5453488826752, 967.6065669059753, 969.8842849731445, 972.419998884201, 974.7531559467316, 976.8233268260956, 978.9653270244598, 981.156849861145, 983.4576888084412, 985.6688449382782, 988.2198028564453, 990.5267899036407, 992.8870198726654, 995.0905230045319, 997.256490945816, 999.5827198028564, 1001.6387898921967, 1003.8559429645538, 1006.1806418895721, 1008.7319920063019, 1011.3197200298309, 1013.912055015564, 1016.5878829956055, 1018.9152739048004, 1021.2979378700256, 1023.703537940979, 1026.2642168998718, 1028.601791858673, 1031.3110389709473, 1033.8543019294739, 1036.2974679470062, 1038.749146938324, 1041.3184368610382, 1043.761953830719, 1046.4490928649902, 1049.098196029663, 1051.6492810249329, 1054.039713859558, 1056.8587248325348, 1059.410353899002, 1061.8291549682617, 1064.4062299728394, 1067.0447318553925, 1069.5492939949036, 1072.1543328762054, 1074.5635948181152, 1076.8833408355713, 1079.4236958026886, 1081.9052708148956, 1084.4437370300293, 1087.030336856842, 1089.6053290367126, 1092.3441288471222, 1094.8981249332428, 1097.24094581604, 1100.0310168266296, 1102.6116738319397, 1105.1315248012543, 1107.4323978424072, 1109.9225199222565, 1112.4210560321808, 1114.9722909927368, 1117.5726218223572, 1120.2428109645844, 1122.8040359020233, 1124.9827208518982, 1127.4678058624268, 1130.06858086586, 1132.4148290157318, 1134.9130330085754, 1137.5585680007935, 1140.296504020691, 1142.6588668823242, 1145.1827898025513, 1147.3161790370941, 1149.7712178230286, 1152.2571189403534, 1154.724575996399, 1157.2082929611206, 1159.9997198581696, 1163.0124928951263, 1165.9401919841766, 1168.318557024002, 1170.9223108291626, 1173.4180250167847, 1176.0080738067627, 1178.566913843155, 1181.063747882843, 1183.6451020240784, 1186.3412029743195, 1188.9941039085388, 1191.6404919624329, 1194.3154509067535, 1196.979651927948, 1199.708771944046, 1202.2550168037415, 1204.9841759204865, 1207.4640028476715, 1209.9744958877563, 1212.4570689201355, 1214.81862783432, 1217.4708259105682, 1220.1595859527588, 1223.2213048934937, 1225.9675829410553, 1228.484493970871, 1231.1856849193573, 1233.78338098526, 1236.4035639762878, 1238.9080619812012, 1241.0693109035492, 1243.3375778198242, 1245.6157999038696, 1248.006817817688, 1250.4906928539276, 1253.5054378509521, 1256.1907849311829, 1258.7539598941803, 1261.3331048488617, 1263.8764119148254, 1266.6595759391785, 1269.1138429641724, 1271.530012845993, 1273.889328956604, 1276.2347919940948, 1278.639307975769, 1280.927397966385, 1284.0044128894806, 1287.1220028400421, 1289.6344769001007, 1292.0526678562164, 1294.695550918579, 1297.199432849884, 1299.6682648658752, 1302.103462934494, 1304.7896139621735, 1307.4586899280548, 1309.9502918720245, 1312.6331379413605, 1315.3422708511353, 1318.0206859111786, 1320.8638470172882, 1323.5244958400726, 1326.1323719024658, 1328.6256649494171, 1331.5724639892578, 1334.3843908309937, 1337.1973419189453, 1339.7809488773346, 1342.1928458213806, 1345.1495549678802, 1347.8173398971558, 1350.3683319091797, 1352.9234149456024, 1355.412276983261, 1357.9848098754883, 1360.5438339710236, 1363.1491060256958, 1365.9183719158173, 1368.7480750083923, 1371.2602949142456, 1373.7147359848022, 1376.1557388305664, 1378.6897230148315, 1381.3217380046844, 1384.2057058811188, 1386.9132339954376, 1389.653627872467, 1392.7175788879395, 1395.562166929245, 1398.2514579296112, 1400.9429109096527, 1403.7378678321838, 1406.4723448753357, 1409.1501610279083, 1411.9131648540497, 1414.7541098594666, 1417.6100039482117, 1420.8499188423157, 1423.8812890052795, 1426.783443927765, 1429.4290969371796, 1432.172523021698, 1435.0541248321533, 1437.9856219291687, 1440.9847729206085, 1443.9582738876343, 1446.7688059806824, 1449.9704158306122, 1452.6653559207916, 1455.4350299835205, 1458.1151139736176, 1460.881583929062, 1464.0331649780273, 1467.0405178070068, 1469.835783958435, 1472.955538034439, 1476.2515878677368, 1479.4401018619537, 1482.2181339263916, 1485.249706029892, 1487.9009609222412, 1490.6063838005066, 1493.3400809764862, 1496.351397037506, 1499.398675918579, 1502.2488958835602, 1505.3536908626556, 1508.4206700325012, 1511.5394558906555, 1514.6989078521729, 1517.3749070167542, 1520.1627659797668, 1523.306977033615, 1526.6104528903961, 1529.9451758861542, 1532.6302678585052, 1535.275545835495, 1537.721431016922, 1540.6471769809723, 1543.5590348243713, 1546.607470035553, 1549.4567918777466, 1552.7658758163452, 1556.3881750106812, 1559.3939118385315, 1562.8964598178864, 1566.515436887741, 1570.144021987915, 1573.1698830127716, 1576.2470989227295, 1578.9594140052795, 1581.7264878749847, 1584.5153369903564, 1587.8269069194794, 1590.643651008606, 1593.445238828659, 1596.2026510238647, 1599.0691788196564, 1601.7717578411102, 1604.5209720134735, 1607.3277218341827, 1609.9988808631897, 1612.9533989429474, 1615.9326379299164, 1619.121927022934, 1622.0284938812256, 1624.9017429351807, 1627.7517080307007, 1630.860242843628, 1633.943099975586, 1636.9022738933563, 1640.052155971527, 1643.1569199562073, 1646.3406569957733, 1649.5251410007477, 1652.7252559661865, 1655.7094349861145, 1658.5039949417114, 1661.237322807312, 1664.0580530166626, 1666.8384640216827, 1669.6686379909515, 1672.5239579677582, 1675.69309091568, 1678.9379279613495, 1682.4656238555908, 1685.4063489437103, 1688.3909389972687, 1691.6037089824677, 1695.0223050117493, 1698.1232569217682, 1701.111228942871, 1704.522050857544, 1707.8027119636536, 1710.672691822052, 1713.4336240291595, 1716.738687992096, 1720.1395359039307, 1723.6570258140564, 1726.4399688243866, 1729.4309649467468, 1732.295037984848, 1735.7266209125519, 1738.5349369049072, 1741.2788689136505, 1743.8882298469543, 1746.5399639606476, 1749.0691378116608, 1751.724336862564, 1754.4323918819427, 1756.9434819221497, 1759.5824828147888, 1762.611214876175, 1765.5603058338165, 1768.6045048236847, 1771.8219299316406, 1775.0012538433075, 1778.0766048431396, 1780.9333798885345, 1783.7622690200806, 1786.9213960170746, 1790.0591759681702, 1793.1625008583069, 1796.1035058498383, 1799.326887845993, 1802.5762929916382, 1805.7262389659882, 1809.0309870243073, 1812.2296328544617, 1815.3423068523407, 1818.3114748001099, 1821.5530378818512, 1824.6749849319458, 1827.7420098781586, 1830.705579996109, 1833.744197845459, 1836.776505947113, 1840.022300004959, 1842.8877849578857, 1845.6558468341827, 1848.6952500343323, 1851.562395811081, 1854.652736902237, 1857.8078389167786, 1860.754534959793, 1863.7897958755493, 1866.7697188854218, 1869.6067810058594, 1872.4533939361572, 1875.2781739234924, 1878.5524969100952, 1881.9137558937073, 1885.2664330005646, 1888.527359008789, 1891.6977849006653, 1895.0323770046234, 1898.3788080215454, 1901.707319021225, 1904.8086178302765, 1908.055300951004, 1911.5094738006592, 1914.899250984192, 1918.0072968006134, 1921.4077208042145, 1924.8923079967499, 1928.3561038970947, 1931.7942569255829, 1935.796327829361, 1939.5258519649506, 1942.732430934906, 1946.0942149162292, 1949.4475758075714, 1952.6423509120941, 1955.6285049915314, 1958.2619969844818, 1961.8101818561554, 1964.8582909107208, 1968.6492710113525, 1972.222636938095, 1975.8497450351715, 1979.43559384346, 1982.686057806015, 1986.4159018993378, 1989.9554889202118, 1993.6650748252869, 1997.017678976059, 2000.205237865448, 2003.0877540111542, 2006.206748008728, 2009.2409868240356, 2012.7346889972687, 2015.9962499141693, 2019.342679977417, 2023.1142299175262, 2026.5112059116364, 2029.9337108135223, 2033.2846519947052, 2036.6900868415833, 2040.127228975296, 2043.2364230155945, 2046.3698949813843, 2049.5942828655243, 2052.866385936737, 2055.8961098194122, 2059.0300748348236, 2062.43155503273, 2065.920415878296, 2069.1225039958954, 2072.3542008399963, 2075.7047049999237, 2078.840646982193, 2082.0305318832397, 2085.374956846237, 2089.0812509059906, 2092.6340408325195, 2096.368626832962, 2099.6302258968353, 2102.774927854538, 2106.0528948307037, 2109.181114912033, 2112.293818950653, 2115.3607869148254, 2118.600107908249, 2121.9425218105316, 2125.0573139190674, 2128.321753025055, 2132.0417609214783, 2135.2494258880615, 2138.507546901703, 2142.092316865921, 2145.4744708538055, 2148.620064973831, 2151.9232819080353, 2155.148887872696, 2158.7364590168, 2162.1494328975677, 2165.596442937851, 2168.7491059303284, 2171.8922488689423, 2175.134001970291, 2178.589746952057, 2181.9552829265594, 2185.0121178627014, 2188.409740924835, 2191.805559873581, 2195.112493991852, 2198.4011759757996, 2201.6326479911804, 2204.9143028259277, 2208.124869823456, 2211.2443108558655, 2214.450229883194, 2217.832804918289, 2221.1039888858795, 2224.7326588630676, 2228.220328807831, 2231.689906835556, 2234.647080898285, 2238.019268989563, 2241.425045967102, 2245.0260639190674, 2248.430454969406, 2251.6177508831024, 2254.7434978485107, 2258.590346813202, 2262.399901866913, 2265.906744003296, 2269.049110889435, 2272.43604183197, 2275.9751279354095, 2279.177881002426, 2283.035562992096, 2286.340754032135, 2289.864271879196, 2293.240634918213, 2296.4024798870087, 2299.7836418151855, 2303.379791021347, 2306.7561299800873, 2310.36630487442, 2313.9394760131836, 2317.151444911957, 2320.4285509586334, 2324.072366952896, 2327.409260034561, 2330.612979888916, 2333.794857978821, 2337.074466943741, 2340.1901059150696, 2343.287451028824, 2346.5704579353333, 2350.1351528167725, 2353.296185016632, 2356.6955749988556, 2359.9544429779053, 2363.1299488544464, 2366.5463659763336, 2370.261396884918, 2373.866483926773, 2377.353299856186, 2380.4288799762726, 2383.7658619880676, 2387.170914888382, 2390.607792854309, 2394.2443590164185, 2397.7933599948883, 2401.4769508838654, 2404.848846912384, 2408.403738975525, 2412.0099580287933, 2415.657289981842, 2419.6936089992523, 2423.6005749702454, 2427.6314868927, 2431.7602128982544, 2435.277391910553, 2438.411763906479, 2441.872560977936, 2445.365263938904, 2449.2506408691406, 2453.03249001503, 2456.5457088947296, 2459.9966559410095, 2463.2359368801117, 2466.3004310131073, 2469.667765855789, 2473.1629338264465, 2476.9559729099274, 2480.2330718040466, 2483.49498796463, 2487.191601037979, 2490.495673894882, 2493.8585159778595, 2497.706874847412, 2501.5092849731445, 2505.2922139167786, 2508.795168876648, 2512.4143648147583, 2516.2365260124207, 2519.7276108264923, 2523.1378309726715, 2526.433748960495, 2529.8710289001465, 2533.403128862381, 2536.791967868805, 2540.3033249378204, 2544.147297859192, 2548.094353914261, 2551.435264825821, 2554.63910984993, 2557.866333961487, 2561.159173965454, 2564.870528936386, 2568.4919469356537, 2571.972263813019, 2575.771271944046, 2579.982486963272, 2583.553689956665, 2586.9720978736877, 2590.1688249111176, 2593.8687109947205, 2597.411388874054, 2600.7793238162994, 2604.3234498500824, 2607.476765871048, 2611.046000957489, 2614.22394990921, 2618.1276059150696, 2621.3482868671417, 2624.7769389152527, 2627.7843668460846, 2630.8633739948273, 2633.9693019390106, 2637.3172879219055, 2640.459259033203, 2643.9293558597565, 2647.8261330127716, 2651.2917449474335]</t>
   </si>
   <si>
     <t xml:space="preserve">LagrangianGradient</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.6518243513673535e6, 1.665381312297116e6, 1.756383755772586e6, 1.7611328553412552e6, 1.7628068615134743e6, 1.7631964224539388e6, 1.7662170491024416e6, 1.766434813111871e6, 1.7681967395255384e6, 1.7692681053351676e6, 1.7726773828320382e6, 1.7752555870522067e6, 1.7765738125556125e6, 1.7770583548769741e6, 1.7787760676773007e6, 1.7804835283893463e6, 1.781621982807487e6, 1.7826636828774973e6, 1.7833732352748073e6, 1.7869409728517109e6, 1.7885502216087375e6, 1.791952254301618e6, 1.7934739110263665e6, 1.7948352285117689e6, 1.7950535783517424e6, 1.7969234481859352e6, 1.7972856781339212e6, 1.801091297296982e6, 1.801188574647982e6, 1.8032441870933145e6, 1.8035942371811983e6, 1.8036103816296011e6, 1.8036930610993e6, 1.8043566050650424e6, 1.8047142966232894e6, 1.80577577328515e6, 1.8060744994585325e6, 1.806124463557159e6, 1.806308420255438e6, 1.8068339577804485e6, 1.8068567275187504e6, 1.8069218133983107e6, 1.8069980673595802e6, 1.8072944427806824e6, 1.8073395057172095e6, 1.8074831386981597e6, 1.8076537564216708e6, 1.8081727545699803e6, 1.8086949407341736e6, 1.809024959017705e6, 1.8097665482318257e6, 1.8099160300041728e6, 1.8099160300041728e6, 1.810043852272999e6, 1.8100028401737825e6, 1.811124857556193e6, 1.8114642590546145e6, 1.8116339228101457e6, 1.8121077559560598e6, 1.8122735123825422e6, 1.8124599134320598e6, 1.8126733434318833e6, 1.8126733434318835e6, 1.8127602243183127e6, 1.8132124214151506e6, 1.8131565585505823e6, 1.8132913451613898e6, 1.8134986841586155e6, 1.81451230123213e6, 1.8146095785831288e6, 1.8148376087208474e6, 1.8150070085346873e6, 1.8151110936814072e6, 1.815139858421361e6, 1.815139858421361e6, 1.815139858421361e6, 1.8152288364495498e6, 1.8153268434841288e6, 1.8153296512369001e6, 1.815608972669326e6, 1.8160882206708563e6, 1.816507483167521e6, 1.8165603470317838e6, 1.816440378146856e6, 1.8166764039834489e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6, 1.8167190052774097e6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941566e6, 1.919477308993592e6, 1.89371970224164e6, 1.8958201881899994e6, 1.9099305774456817e6, 1.90040249903029e6, 1.9007320723125231e6, 1.8839535148946866e6, 1.8891186351494435e6, 1.8949386596644847e6, 1.9067046501815666e6, 1.90851586706978e6, 1.874666238257998e6, 1.87611672423065e6, 1.8999973599976825e6, 1.8713141131868295e6, 1.8396475817312223e6, 1.90670469035238e6, 1.8508051387279488e6, 1.84582850986437e6, 1.8689349254995903e6, 1.8446495583063785e6, 1.9159095595387546e6, 1.8810254025277372e6, 1.8701917816331813e6, 1.847686476632762e6, 1.863050827551882e6, 1.8818484732428e6, 1.849925833853117e6, 1.8508925192602559e6, 1.8742667399324893e6, 1.8340408485196459e6, 1.886450191434473e6, 1.8340939225835835e6, 1.8648988372260898e6, 1.842227894400236e6, 1.8936813297298106e6, 1.8332484827633451e6, 1.8618892952851395e6, 1.8499453445204434e6, 1.8474020729997966e6, 1.8346774966272332e6, 1.8526287017886543e6, 1.8294599797363055e6, 1.8442495706960235e6, 1.8638268238231677e6, 1.8428435717943783e6, 1.8617189679092502e6, 1.8415863035501495e6, 1.8369677796130048e6, 1.8699543610577437e6, 1.8605009881031609e6, 1.839541137849115e6, 1.8433292471543776e6, 1.9041209104681527e6, 1.8764495086534887e6, 1.8507117322279655e6, 1.8386075138180384e6, 1.8444197424579964e6, 1.8470910186591547e6, 1.843658965243826e6, 1.8423549071334603e6, 1.848382144693955e6, 1.8833084618691106e6, 1.8291107040525873e6, 1.8555112814230423e6, 1.8644718789869824e6, 1.8540033148664085e6, 1.8416962762726985e6, 1.8355279679457962e6, 1.8455760124185744e6, 1.8514972571640222e6, 1.863480402888417e6, 1.8368931391384515e6, 1.8446568901950757e6, 1.8350081999122223e6, 1.8332793619248017e6, 1.8270900462159256e6, 1.845177922967551e6, 1.8317372647101118e6, 1.832051145876589e6, 1.8293633099857124e6, 1.8409755862116774e6, 1.8647605202024884e6, 1.829407022791947e6, 1.8293608460609957e6, 1.8293608460609957e6, 1.8294238669826684e6, 1.8293608460609957e6, 1.8294238669826684e6, 1.8293259717515686e6, 1.829173485174902e6, 1.829173485174902e6, 1.829173485174902e6, 1.8293608460609957e6, 1.8292713804060013e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6, 1.829173485174902e6, 1.8292713804060013e6]</t>
+    <t xml:space="preserve">[1.651871418609248e6, 1.6653930106214131e6, 1.7560395892607088e6, 1.761453389632145e6, 1.7615250264398432e6, 1.7622888461253198e6, 1.764963837514393e6, 1.7657298483357704e6, 1.7675273364985003e6, 1.7687852518032482e6, 1.769163078788391e6, 1.7706313288361947e6, 1.773431645862056e6, 1.7735611856928503e6, 1.7737534804016198e6, 1.7766011736784286e6, 1.7856502028944232e6, 1.786632395222021e6, 1.7868037371112457e6, 1.7901842990444985e6, 1.7908371201612111e6, 1.7938589092936341e6, 1.7942945450598295e6, 1.7956442750030071e6, 1.7969739466349292e6, 1.7970712239859293e6, 1.797442303384258e6, 1.7976401570907566e6, 1.798211686585865e6, 1.7983621455808189e6, 1.8011367662302835e6, 1.8011644751316556e6, 1.802830869305883e6, 1.8036872224017128e6, 1.804341790132528e6, 1.8055755936317875e6, 1.8058155883657017e6, 1.805766098035365e6, 1.805972160337902e6, 1.8064427858696543e6, 1.8074176551208494e6, 1.807532546240845e6, 1.8087941048815781e6, 1.8089030791456685e6, 1.8094544347378695e6, 1.8094433677012902e6, 1.80970291204421e6, 1.8098205787895217e6, 1.8099295532825217e6, 1.8101140109799595e6, 1.8102636187734683e6, 1.8103541703679685e6, 1.8108138062350017e6, 1.8109167890575554e6, 1.8111413659072805e6, 1.8114193537610644e6, 1.8116724490119747e6, 1.8119634162820743e6, 1.812209968698641e6, 1.8120375564369743e6, 1.8120375564369743e6, 1.8122690561375294e6, 1.8125529963305017e6, 1.8139566611357497e6, 1.8140539384867498e6, 1.8145386305665206e6, 1.8144060959627498e6, 1.8144825281592552e6, 1.8144060959627498e6, 1.8147712033877478e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147712033877496e6, 1.8147720144748837e6, 1.815013664758868e6, 1.8155455879264497e6, 1.8155455879264497e6, 1.8155455879264497e6, 1.8156434998718163e6, 1.8156543859301573e6, 1.8156543859301573e6, 1.8164887690167418e6, 1.8165475890010851e6, 1.8165860463677421e6, 1.8168651094111956e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6, 1.8168651094111954e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.844825859920311e6, 1.923591527294157e6, 1.919477308993592e6, 1.894556613062513e6, 1.940803580161283e6, 1.8963866692813763e6, 1.9051676078772596e6, 1.901848538899502e6, 1.8937910079285037e6, 1.8868143758796847e6, 1.8832093561036084e6, 1.9820145449887705e6, 1.912196182279984e6, 1.909167051272673e6, 1.8505074661150493e6, 1.8531056165736832e6, 1.8741392243211872e6, 1.8629978811400176e6, 1.854116651415149e6, 1.872507313646131e6, 1.8621876272406748e6, 1.8462005776208767e6, 1.8416794853626292e6, 1.8320444793413861e6, 1.8581748580553776e6, 1.8551520667672951e6, 1.859056085309948e6, 1.8510854444909522e6, 1.8767822057705505e6, 1.8743616271247847e6, 1.8645602849394355e6, 1.8612381378545158e6, 1.8374619250006087e6, 1.8497619830146024e6, 1.8643132756748388e6, 1.8427791661253853e6, 1.858927707641118e6, 1.862949954403911e6, 1.8496170809588798e6, 1.8466776309480926e6, 1.8523362009641754e6, 1.8419335594013582e6, 1.9139264830011788e6, 1.8666736574873987e6, 1.8487001318203972e6, 1.8509826431544304e6, 1.8456396783659954e6, 1.8291612330230891e6, 1.8356436447624627e6, 1.8676573004473445e6, 1.862370797164561e6, 1.8439332032981676e6, 1.8522985847627686e6, 1.8330904883724328e6, 1.8399407240152902e6, 1.850111544985865e6, 1.846944627705801e6, 1.8452269333853463e6, 1.8574964370989234e6, 1.8341554032297304e6, 1.8301547823949254e6, 1.8443990343635443e6, 1.8363711411730691e6, 1.8780086511540075e6, 1.8384298124718985e6, 1.841226834236962e6, 1.8497863051805908e6, 1.832782677836655e6, 1.8393688814850475e6, 1.8538755318421277e6, 1.8326522851807706e6, 1.8455796506214605e6, 1.8320409842798181e6, 1.8389311734726334e6, 1.834943493353055e6, 1.8290989108008135e6, 1.8388208793440654e6, 1.8323182022823982e6, 1.8665059724458975e6, 1.8307076847256639e6, 1.8519575903631134e6, 1.8292866367597946e6, 1.8553011996702033e6, 1.8478722588490874e6, 1.828994221640031e6, 1.8456407481251748e6, 1.8693882889891143e6, 1.8592225341986993e6, 1.8357208623521582e6, 1.8289091234147784e6, 1.8293404000284567e6, 1.8293488413515843e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6, 1.8293388253709266e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.5786018371582031, 3.5907437801361084, 7.290550947189331, 8.980089902877808, 11.547634840011597, 13.595641851425171, 15.56404995918274, 17.417528867721558, 18.976240873336792, 20.8192458152771, 22.145401000976562, 24.200052976608276, 26.20512080192566, 27.73187279701233, 28.828617811203003, 29.983354806900024, 31.055262804031372, 32.20572090148926, 33.30303597450256, 34.81355690956116, 36.23726677894592, 37.41624593734741, 38.61310601234436, 39.608136892318726, 40.750624895095825, 41.799219846725464, 44.64375185966492, 46.321372985839844, 47.75894284248352, 48.79060077667236, 50.028679847717285, 52.86759901046753, 53.862754821777344, 55.18510389328003, 56.65889000892639, 57.74891400337219, 58.899698972702026, 60.154947996139526, 61.37483286857605, 62.68456292152405, 63.94369983673096, 65.27397680282593, 67.35247993469238, 68.6610198020935, 69.96699500083923, 71.18954396247864, 72.23795485496521, 73.4246768951416, 74.5034430027008, 75.98268580436707, 77.43753480911255, 78.50488185882568, 79.81295680999756, 80.92785477638245, 81.9238429069519, 83.1792938709259, 84.28539681434631, 85.4080319404602, 86.856440782547, 87.98869800567627, 89.16467690467834, 90.09757399559021, 91.13497686386108, 92.63930487632751, 93.77016997337341, 94.93200087547302, 96.26505589485168, 97.32398200035095, 98.3187198638916, 99.5455379486084, 100.59104490280151, 101.78907895088196, 102.8649377822876, 104.01753187179565, 105.02614879608154, 106.07696890830994, 107.08619999885559, 108.1223669052124, 109.33144998550415, 110.37404298782349, 111.71836185455322, 112.83333277702332, 114.0314199924469, 115.24079489707947, 116.35472178459167, 117.44781279563904, 118.80752897262573, 119.94757080078125, 121.05586886405945, 122.1678409576416, 123.31549596786499, 124.4202709197998, 125.52502179145813, 126.64887690544128, 127.75711488723755, 128.86352586746216, 129.9970989227295, 131.09458184242249, 132.19665384292603, 133.29669785499573, 134.41422986984253, 135.52778887748718, 136.65114188194275, 137.77483081817627, 138.9226529598236, 140.0240888595581, 141.12283396720886, 142.23335886001587, 143.36385083198547, 144.49547600746155, 145.6183888912201, 146.71805691719055, 147.83548378944397, 148.9494137763977, 150.06470680236816, 151.19063687324524, 152.3048059940338, 153.41945695877075, 154.5242998600006, 155.65308094024658, 156.78191900253296, 157.89938688278198, 159.015695810318, 160.13246178627014, 161.2438988685608, 162.38764691352844, 163.5210349559784, 164.64775681495667, 165.76766896247864, 166.89012384414673, 168.01183891296387, 169.12253999710083, 170.2483868598938, 171.36794900894165, 172.47087693214417, 173.59918785095215, 174.72595500946045, 175.8660318851471, 176.99975299835205, 178.2101228237152, 179.34865379333496, 180.4721179008484, 181.69033479690552, 182.8153247833252, 184.0977427959442, 185.2413649559021, 186.37548398971558, 187.5350158214569, 188.66314888000488, 189.80880284309387, 190.93863677978516, 192.0889208316803, 193.2213158607483, 194.3846709728241, 195.5198359489441, 196.6906487941742, 197.81890678405762, 198.98009395599365, 200.12658596038818, 201.2725179195404, 202.41598081588745, 203.57187581062317, 204.70960593223572, 205.8394899368286, 207.00784277915955, 208.14528894424438, 209.30528593063354, 210.44634795188904, 211.68486881256104, 212.86766290664673, 214.02746987342834, 215.19713187217712, 216.3655309677124, 217.51925778388977, 218.6815149784088, 219.87942600250244, 221.03612184524536, 222.203941822052, 223.35422897338867, 224.51148390769958, 225.63997077941895, 226.80034589767456, 227.95250582695007, 229.09338879585266, 230.24302697181702, 231.39674878120422, 232.5540599822998, 233.6837728023529, 234.8451988697052, 236.00502586364746, 237.163507938385, 238.30440497398376, 239.461749792099, 240.60241079330444, 241.75888395309448, 242.91746282577515, 244.07683992385864, 245.22769689559937, 246.38005590438843, 247.55735778808594, 248.7435178756714, 249.89214992523193, 251.062668800354, 252.21358489990234, 253.38214492797852, 254.56502199172974, 255.72821283340454, 256.8704779148102, 258.0298538208008, 259.20163798332214, 260.3595278263092, 261.53174686431885, 262.6813678741455, 263.8463468551636, 265.00796484947205, 266.1927947998047, 267.33916091918945, 268.4952600002289, 269.66129994392395, 270.8097298145294, 271.9746367931366, 273.1616208553314, 274.36150789260864, 275.5318958759308, 276.69468879699707, 277.8453438282013, 279.00044679641724, 280.17707800865173, 281.3884379863739, 282.5512709617615, 283.73855090141296, 284.89813590049744, 286.1117799282074, 287.3513638973236, 288.5708818435669, 289.77251291275024, 290.9933428764343, 292.21013379096985, 293.4170808792114, 294.6398649215698, 295.8980839252472, 297.22234082221985, 298.6212999820709, 299.829580783844, 301.04218792915344, 302.2300109863281, 303.45083498954773, 304.66113686561584, 305.8697669506073, 307.0829529762268, 308.3000497817993, 309.4917459487915, 310.69567799568176, 311.89431285858154, 313.0959949493408, 314.33399391174316, 315.5209798812866, 316.7405068874359, 317.925794839859, 319.13507199287415, 320.3473219871521, 321.55573987960815, 322.74543285369873, 323.9360599517822, 325.1454129219055, 326.33386278152466, 327.5151379108429, 328.7059488296509, 329.9008820056915, 331.09599781036377, 332.28304982185364, 333.4880700111389, 334.6949269771576, 335.91623878479004, 337.1199288368225, 338.3192558288574, 339.51528096199036, 340.7425858974457, 341.94644379615784, 343.2024428844452, 344.39402985572815, 345.62611389160156, 346.8344488143921, 348.03284788131714, 349.24660181999207, 350.4424657821655, 351.65212392807007, 352.8819148540497, 354.0901689529419, 355.28299593925476, 356.48338079452515, 357.6818778514862, 358.8987169265747, 360.10941886901855, 361.3096899986267, 362.5145688056946, 363.7102358341217, 364.9241178035736, 366.1479218006134, 367.39258885383606, 368.6100649833679, 369.824355840683, 371.0499107837677, 372.27150893211365, 373.4935669898987, 374.71186780929565, 375.9396708011627, 377.190171957016, 378.42077684402466, 379.6391267776489, 380.8660559654236, 382.0894989967346, 383.33679699897766, 384.58085083961487, 385.83820700645447, 387.1423988342285, 388.38384890556335, 389.6112678050995, 390.837299823761, 392.09975481033325, 393.3399519920349, 394.58400893211365, 395.90404987335205, 397.32148480415344, 398.5726978778839, 399.83252477645874, 401.0848639011383, 402.3543448448181, 403.62020683288574, 404.8899099826813, 406.1485347747803, 407.4326570034027, 408.68722581863403, 409.9399719238281, 411.1770598888397, 412.43027687072754, 413.6770718097687, 414.9575688838959, 416.21034383773804, 417.5040647983551, 418.8305959701538, 420.0839328765869, 421.3416199684143, 422.5938699245453, 423.87857389450073, 425.1282329559326, 426.40872383117676, 427.708655834198, 428.96435379981995, 430.2233510017395, 431.4974420070648, 432.7504367828369, 434.0109009742737, 435.2884418964386, 436.55854988098145, 437.8763117790222, 439.1341350078583, 440.40816378593445, 441.6708719730377, 442.9273428916931, 444.22881388664246, 445.5038139820099, 446.7946720123291, 448.1548709869385, 449.45159888267517, 450.8040609359741, 452.14994597435, 453.43602299690247, 454.72626185417175, 456.03355598449707, 457.30749583244324, 458.59676790237427, 459.9047169685364, 461.17652583122253, 462.4835457801819, 463.80088782310486, 465.15243577957153, 466.52103900909424, 467.86532282829285, 469.20300698280334, 470.5108788013458, 471.8144679069519, 473.1280999183655, 474.4459698200226, 475.76886677742004, 477.0551609992981, 478.3574459552765, 479.65396189689636, 480.94004487991333, 482.24306893348694, 483.53096079826355, 484.8363878726959, 486.14013385772705, 487.4675199985504, 488.75742387771606, 490.06112790107727, 491.35402488708496, 492.64185190200806, 493.95047092437744, 495.2583417892456, 496.567430973053, 497.8774199485779, 499.17460799217224, 500.4801049232483, 501.7892699241638, 503.0917329788208, 504.404935836792, 505.726735830307, 507.04008197784424, 508.43607091903687, 509.9073028564453, 511.220871925354, 512.5910968780518, 513.907283782959, 515.2444689273834, 516.5883519649506, 517.945592880249, 519.2809588909149, 520.6572449207306, 521.9830458164215, 523.3013908863068, 524.6330788135529, 525.9700939655304, 527.3014907836914, 528.6399037837982, 529.9695439338684, 531.2854778766632, 532.6129479408264, 533.9628448486328, 535.3067109584808, 536.6424329280853, 537.9585208892822, 539.2862348556519, 540.6212329864502, 541.9676079750061, 543.3327159881592, 544.6491169929504, 545.9960038661957, 547.3163959980011, 548.7436978816986, 550.0953288078308, 551.4513969421387, 552.8329358100891, 554.1658358573914, 555.5220198631287, 556.8769228458405, 558.2546107769012, 559.5746159553528, 560.9345898628235, 562.2945709228516, 563.6255459785461, 564.9620568752289, 566.2902359962463, 567.6370868682861, 568.9668459892273, 570.3366839885712, 571.6762118339539, 573.0396299362183, 574.4395999908447, 575.7895948886871, 577.1342978477478, 578.4779949188232, 579.8513119220734, 581.1964449882507, 582.5949227809906, 584.0043649673462, 585.4296178817749, 586.8207969665527, 588.2026557922363, 589.6040978431702, 590.9901299476624, 592.3622598648071, 593.7510938644409, 595.1317667961121, 596.5682768821716, 597.9780788421631, 599.352187871933, 600.676038980484, 601.9729208946228, 603.3013648986816, 604.6148409843445, 605.9262928962708, 607.2229888439178, 608.6273488998413, 610.085944890976, 611.4096047878265, 612.7283418178558, 614.0414278507233, 615.3700108528137, 616.6884667873383, 618.0013589859009, 619.3132688999176, 620.6266257762909, 621.9591999053955, 623.2757837772369, 624.5946989059448, 625.9111948013306, 627.2249088287354, 628.540787935257, 629.8515508174896, 631.181578874588, 632.4981729984283, 633.8397159576416, 635.1649038791656, 636.572515964508, 637.8933448791504, 639.2323877811432, 640.5640540122986, 641.8882257938385, 643.2195298671722, 644.5548408031464, 645.8760550022125, 647.2062718868256, 648.5458388328552, 649.8719198703766, 651.2291870117188, 652.5729739665985, 653.894544839859, 655.2250618934631, 656.5583148002625, 657.919095993042, 659.2702589035034, 660.6004629135132, 661.9235618114471, 663.2662317752838, 664.5991659164429, 665.9442429542542, 667.2767508029938, 668.6173059940338, 669.9426457881927, 671.308995962143, 672.6462688446045, 673.9788959026337, 675.336639881134, 676.6927559375763, 678.0298528671265, 679.3721978664398, 680.7160439491272, 682.0598728656769, 683.4037809371948, 684.7411530017853, 686.1232998371124, 687.4741089344025, 688.8159458637238, 690.1636598110199, 691.5370478630066, 692.9401698112488, 694.2926969528198, 695.6647119522095, 697.0253388881683, 698.3973808288574, 699.7499809265137, 701.1142568588257, 702.4615218639374, 703.8221819400787, 705.2724189758301, 706.7935009002686, 708.1747369766235, 709.5425038337708, 710.9177849292755, 712.2919018268585, 713.6660659313202, 715.0521709918976, 716.4469439983368, 717.8210339546204, 719.2066178321838, 720.586452960968, 721.9731249809265, 723.350686788559, 724.7332108020782, 726.1163527965546, 727.5000178813934, 728.8989369869232, 730.2805788516998, 731.6642718315125, 733.0462548732758, 734.4377899169922, 735.8451910018921, 737.2383937835693, 738.6488609313965, 740.0315389633179, 741.4019138813019, 742.81098985672, 744.2071897983551, 745.6096379756927, 747.0133187770844, 748.423889875412, 749.8143908977509, 751.2071058750153, 752.5927488803864, 753.9732718467712, 755.3803060054779, 756.8075578212738, 758.2413778305054, 759.6375138759613, 761.0963649749756, 762.5134329795837, 763.9132339954376, 765.3233528137207, 766.7573828697205, 768.155622959137, 769.5581059455872, 770.9599769115448, 772.4064538478851, 773.8635308742523, 775.2723019123077, 776.695060968399, 778.0924789905548, 779.4973838329315, 780.9131238460541, 782.3182909488678, 783.7376909255981, 785.1505508422852, 786.5715389251709, 788.014476776123, 789.4281659126282, 790.8432998657227, 792.2498579025269, 793.68017578125, 795.0980498790741, 796.5093669891357, 797.9434559345245, 799.3619878292084, 801.0276849269867, 802.4733438491821, 803.9038779735565, 805.3491129875183, 806.8248808383942, 808.2752079963684, 809.7138588428497, 811.1594698429108, 812.6071448326111, 814.0440008640289, 815.4821848869324, 816.9809658527374, 818.419853925705, 819.8632400035858, 821.3009538650513, 822.7513217926025, 824.197595834732, 825.653571844101, 827.1183698177338, 828.5686278343201, 830.0232899188995, 831.4659729003906, 832.910404920578, 834.3716928958893, 835.823362827301, 837.2846179008484, 838.7349908351898, 840.2026598453522, 841.6689758300781, 843.1195387840271, 844.5947098731995, 846.080002784729, 847.5661549568176, 849.0258989334106, 850.4738848209381, 851.9429159164429, 853.3975479602814, 854.8572998046875, 856.3184869289398, 857.7749857902527, 859.237174987793, 860.7040297985077, 862.1639168262482, 863.6540629863739, 865.1298389434814, 866.6031968593597, 868.0711619853973, 869.5412428379059, 871.0115358829498, 872.4954299926758, 873.9658398628235, 875.4853417873383, 876.9837667942047, 878.4665768146515, 879.9416909217834, 881.4053440093994, 882.8831188678741, 884.3632609844208, 885.8677108287811, 887.6012949943542, 889.0989890098572, 890.589605808258, 892.0748670101166, 893.5620069503784, 895.050539970398, 896.5656929016113, 898.0731089115143, 899.6313328742981, 901.1375138759613, 902.6385638713837, 904.1405439376831, 905.642758846283, 907.1457109451294, 908.6591680049896, 910.1583788394928, 911.6552519798279, 913.1662709712982, 914.6641569137573, 916.170551776886, 917.6824359893799, 919.1999487876892, 920.7026319503784, 922.2048988342285, 923.7112538814545, 925.2217738628387, 926.7300548553467, 928.2482709884644, 929.7556138038635, 931.284029006958, 932.8314938545227, 934.3575029373169, 935.8868968486786, 937.4017519950867, 938.910092830658, 940.4210298061371, 941.9394648075104, 943.4520688056946, 944.9671308994293, 946.5214278697968, 948.0479118824005, 949.578537940979, 951.1076548099518, 952.6310648918152, 954.157105922699, 955.6807808876038, 957.2490878105164, 958.7810339927673, 960.3090698719025, 961.8339438438416, 963.3581998348236, 964.8802349567413, 966.4286358356476, 967.972737789154, 969.501072883606, 971.0303997993469, 972.7937989234924, 974.3411159515381, 975.8781278133392, 977.4352099895477, 978.9883999824524, 980.5319559574127, 982.0890698432922, 983.6331708431244, 985.1921498775482, 986.7533857822418, 988.3114149570465, 989.8621189594269, 991.417778968811, 992.9663648605347, 994.5252277851105, 996.0836498737335, 997.6503069400787, 999.2104640007019, 1000.8163239955902, 1002.3862090110779, 1003.9478418827057, 1005.5086917877197, 1007.0802159309387, 1008.6494448184967, 1010.2141778469086, 1011.7888159751892, 1013.3556518554688, 1014.9230539798737, 1016.5161609649658, 1018.102047920227, 1019.6713027954102, 1021.2516798973083, 1022.8251059055328, 1024.4000267982483, 1025.9722218513489, 1027.5993700027466, 1029.175498008728, 1030.7487239837646, 1032.3245480060577, 1033.902704000473, 1035.4919459819794, 1037.089460849762, 1038.6707718372345, 1040.2511069774628, 1041.8321869373322, 1043.426085948944, 1045.024736881256, 1046.6253979206085, 1048.2159450054169, 1049.8052117824554, 1051.3966398239136, 1052.990643978119, 1054.5885457992554, 1056.1955969333649, 1057.8051629066467, 1059.4066109657288, 1061.006199836731, 1062.6210808753967, 1064.3102719783783, 1066.068836927414, 1067.701320886612, 1069.3237488269806, 1070.946702003479, 1072.6106839179993, 1074.2411658763885, 1075.8618128299713, 1077.517390012741, 1079.1543719768524, 1080.7785367965698, 1082.411950826645, 1084.0443058013916, 1085.6713619232178, 1087.345191001892, 1088.9869968891144, 1090.627769947052, 1092.2673988342285, 1093.903375864029, 1095.5466799736023, 1097.2030069828033, 1098.852136850357, 1100.4928197860718, 1102.143501996994, 1103.7862010002136, 1105.437865972519, 1107.0854289531708, 1108.7389588356018, 1110.384971857071, 1112.0456748008728, 1113.6926009654999, 1115.3472797870636, 1117.010125875473, 1118.6632168293, 1120.3253028392792, 1121.9792568683624, 1123.6327447891235, 1125.2970259189606, 1126.9639999866486, 1128.6241388320923, 1130.3029358386993, 1131.9776668548584, 1133.6532609462738, 1135.3375837802887, 1137.0126659870148, 1138.7318828105927, 1140.4175279140472, 1142.094102859497, 1143.7701499462128, 1145.4584708213806, 1147.1666769981384, 1148.8675689697266, 1150.564143896103, 1152.2542009353638, 1153.9450688362122, 1155.6340839862823, 1157.3687539100647, 1159.1624608039856, 1161.0089128017426, 1162.7415750026703, 1164.459969997406, 1166.184122800827, 1167.930261850357, 1169.6538197994232, 1171.4254868030548, 1173.1574928760529, 1174.8929908275604, 1176.638261795044, 1178.3813478946686, 1180.1161518096924, 1181.8589940071106, 1183.602059841156, 1185.3454508781433, 1187.089852809906, 1188.8498919010162, 1190.6008839607239, 1192.3440799713135, 1194.09858584404, 1195.8520498275757, 1197.6026358604431, 1199.3604388237, 1201.111764907837, 1202.8699069023132, 1204.6358058452606, 1206.3930068016052, 1208.1542918682098, 1209.9138967990875, 1211.6818308830261, 1213.43985080719, 1215.2109589576721, 1216.9839169979095, 1218.778375864029, 1220.5436217784882, 1222.3212368488312, 1224.089509010315, 1225.8659119606018, 1227.668406009674, 1229.4622688293457, 1231.2348759174347, 1233.022540807724, 1234.8006529808044, 1236.5914559364319, 1238.3967549800873, 1240.2103929519653, 1242.2540459632874, 1244.061233997345, 1245.8609268665314, 1247.6708419322968, 1249.4785859584808, 1251.2884848117828, 1253.0941309928894, 1254.9162738323212, 1256.725017786026, 1258.561679840088, 1260.3869979381561, 1262.207091808319, 1264.02841091156, 1265.847277879715, 1267.6741299629211, 1269.4967319965363, 1271.3196358680725, 1273.134524822235, 1274.960334777832, 1276.7828669548035, 1278.6097078323364, 1280.428394794464, 1282.2585968971252, 1284.0892419815063, 1285.9220578670502, 1287.7669138908386, 1289.61128282547, 1291.4476418495178, 1293.285898923874, 1295.1169137954712, 1296.9563858509064, 1298.846391916275, 1300.6790058612823, 1302.5259499549866, 1304.3632409572601, 1306.208200931549, 1308.0731618404388, 1309.9141190052032, 1311.7610909938812, 1313.6035068035126, 1315.4520468711853, 1317.304144859314, 1319.1673848628998, 1321.023230791092, 1322.954866886139, 1324.9733979701996, 1326.83624792099, 1328.7090799808502, 1330.5755009651184, 1332.446214914322, 1334.3149809837341, 1336.18163895607, 1338.0625948905945, 1339.9404277801514, 1341.817302942276, 1343.6935338974, 1345.573754787445, 1347.4681499004364, 1349.3677117824554, 1351.2488420009613, 1353.1326949596405, 1355.013023853302, 1356.8954858779907, 1358.826632976532, 1360.7154178619385, 1362.6067578792572, 1364.4972529411316, 1366.3852908611298, 1368.2994158267975, 1370.1871938705444, 1372.102166891098, 1374.0019488334656, 1375.897882938385, 1377.8033769130707, 1379.7598378658295, 1381.6515808105469, 1383.5453748703003, 1385.431310892105, 1387.3292667865753, 1389.2448348999023, 1391.1370329856873, 1393.0398399829865, 1394.9453258514404, 1396.8412318229675, 1398.7536189556122, 1400.659786939621, 1402.5601959228516, 1404.6988558769226, 1406.6298768520355, 1408.5488398075104, 1410.4770729541779, 1412.4622387886047, 1414.3810958862305, 1416.3118720054626, 1418.259572982788, 1420.2039258480072, 1422.1345808506012, 1424.0637109279633, 1425.9936518669128, 1427.9557948112488]</t>
   </si>
   <si>
     <t xml:space="preserve">ContinuousRelaxation</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.5501780615840121e6, 1.575561930827464e6, 1.6785311306715666e6, 1.6806601370430358e6, 1.6981378541338865e6, 1.6989115015069875e6, 1.7052294794488396e6, 1.7067717300408185e6, 1.7180261323612323e6, 1.7189562245976385e6, 1.7202875785285064e6, 1.723170554805087e6, 1.7288698238587566e6, 1.72879468894809e6, 1.7386774942397596e6, 1.7417096730566523e6, 1.7448860613222348e6, 1.7472647689520286e6, 1.7580784431836572e6, 1.760546991820821e6, 1.7609995155314677e6, 1.7612439050197187e6, 1.7628238538893645e6, 1.762761949840902e6, 1.763114107316902e6, 1.7634659838796977e6, 1.7645418144043568e6, 1.7654061143458057e6, 1.7655700274407363e6, 1.766345647614446e6, 1.7671862029844173e6, 1.7680690907823166e6, 1.7698275212481942e6, 1.7700755295514376e6, 1.7709586031859068e6, 1.7712359715447815e6, 1.7719799372776304e6, 1.7719799372776311e6, 1.7720777625461468e6, 1.7723265482696074e6, 1.7727089892036598e6, 1.7741747732240672e6, 1.7742720505750675e6, 1.7748769581797137e6, 1.7750253366837169e6, 1.775286999200772e6, 1.776464519817161e6, 1.7766389510465865e6, 1.776896702569913e6, 1.776984652585708e6, 1.7770054820033312e6, 1.7773774692404473e6, 1.7774031466439557e6, 1.7774043846158264e6, 1.7776104748638351e6, 1.7778130098272143e6, 1.7779446901880542e6, 1.777865860759042e6, 1.7779772077986836e6, 1.7779772077986836e6, 1.7780769583717368e6, 1.778178010782482e6, 1.7783138839380795e6, 1.7784866924506337e6, 1.7784438959404086e6, 1.7786066908046308e6, 1.778683123106017e6, 1.778683123106017e6, 1.7787963578483162e6, 1.7788191012777886e6, 1.77968396569266e6, 1.7799311212515186e6, 1.7805296713178111e6, 1.7803593363468125e6, 1.7803593363468125e6, 1.7803593363468125e6, 1.780534560804225e6, 1.7809208809964966e6, 1.7809920187112489e6, 1.7809920187112489e6, 1.7809920187112489e6, 1.7809920187112489e6, 1.7809920187112489e6, 1.7809920187112489e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811604209370431e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7811953188504418e6, 1.7813618342552977e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6, 1.7813618342553005e6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941575e6, 1.935608287563637e6, 1.8979115987009243e6, 1.9338432085310626e6, 1.889156881510664e6, 1.91167947270936e6, 1.9214856208077562e6, 1.9005501295915127e6, 1.896106213390808e6, 1.903305253628029e6, 1.8511197355410568e6, 1.884446966612503e6, 1.9275242883371771e6, 1.8790167887538297e6, 1.9114485286744663e6, 1.9039854039318343e6, 1.851322484046154e6, 1.8757010047633706e6, 1.880577991260542e6, 1.9090399460146006e6, 1.8609584286844204e6, 1.8614545742348868e6, 1.853456207280976e6, 1.8388970668916495e6, 1.8502406366196482e6, 1.8530848573566705e6, 1.8607418887924396e6, 1.880423610601938e6, 1.8292363732288193e6, 1.8982379758969655e6, 1.8831153611724651e6, 1.8677114540904923e6, 1.8388192800985968e6, 1.8608813777662774e6, 1.8424485746673725e6, 1.85082556406308e6, 1.8602605529775426e6, 1.8625905524990533e6, 1.8291783369314552e6, 1.8513813799387298e6, 1.889625619854091e6, 1.8447377372083797e6, 1.8554993765558887e6, 1.8684308657892884e6, 1.851368065768243e6, 1.8485257835730475e6, 1.8572589908740504e6, 1.8724894319363886e6, 1.8478945741106e6, 1.8850487784309455e6, 1.8378050410898798e6, 1.846130879055144e6, 1.8318131389062519e6, 1.8336718880759424e6, 1.8489101765048772e6, 1.8315271886301434e6, 1.8781258943346485e6, 1.8554883880491883e6, 1.8398419776196831e6, 1.891186973194829e6, 1.836399678745744e6, 1.863806918738112e6, 1.833767367747201e6, 1.844817022964413e6, 1.861171510777618e6, 1.851483052180079e6, 1.8541376830988454e6, 1.8559457424863798e6, 1.8345823142261964e6, 1.8558552821644626e6, 1.8988547646003088e6, 1.8401744403082859e6, 1.8273622559165626e6, 1.8369652059834988e6, 1.8299843258198092e6, 1.8645805921153703e6, 1.862578495161269e6, 1.831033016223132e6, 1.841419501011938e6, 1.8416645226486835e6, 1.8811949665573514e6, 1.8340981568311942e6, 1.8277510142837104e6, 1.8585546193667299e6, 1.8349751020580407e6, 1.8308420770144265e6, 1.8304169539165928e6, 1.8474417010944088e6, 1.9045316437717758e6, 1.844138459458835e6, 1.8334866442075341e6, 1.8716224266474717e6, 1.8475245802575038e6, 1.8276931758753776e6, 1.8369536917195816e6, 1.8309471116816334e6, 1.8365301686538544e6, 1.8309279990869241e6, 1.8306049191642606e6, 1.862386835868676e6, 1.8719340745181188e6, 1.828057217633011e6, 1.8345353100138928e6, 1.8309738527045923e6, 1.8381430199616875e6, 1.851262887601793e6, 1.8342402850233933e6, 1.8273702419643768e6, 1.8332455883772227e6, 1.841041011875373e6, 1.8272676077482298e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6, 1.8271410523922301e6]</t>
+    <t xml:space="preserve">[1.5501780615840121e6, 1.575561930827464e6, 1.6785311306715666e6, 1.6806601370430358e6, 1.697999941326784e6, 1.6989154027495552e6, 1.7046413612845172e6, 1.7063240342469483e6, 1.7334950442099823e6, 1.7379903752589137e6, 1.7386897894529882e6, 1.7406583855644786e6, 1.7418864578669604e6, 1.742438161232549e6, 1.7464552126954147e6, 1.7466270042342036e6, 1.749196350807319e6, 1.7491212158966523e6, 1.749473373372652e6, 1.7500735048969816e6, 1.7525666643922515e6, 1.7585028446125716e6, 1.758829403520075e6, 1.7607041960414413e6, 1.7625547857684614e6, 1.7632186595514922e6, 1.7657286613576843e6, 1.765972135945159e6, 1.765972135945159e6, 1.7663605070813445e6, 1.7667132441024687e6, 1.768626920776453e6, 1.7687982707910247e6, 1.768895548142025e6, 1.769081537844326e6, 1.769145760898665e6, 1.7699617889368536e6, 1.7707560073885615e6, 1.7709613855718249e6, 1.7720364538553252e6, 1.7720145453517092e6, 1.7724016933400193e6, 1.772878649988335e6, 1.7728981815094794e6, 1.7731427665277703e6, 1.7745974285919173e6, 1.7747951987332003e6, 1.7753736818384835e6, 1.7760614592998582e6, 1.7765232946824653e6, 1.7772698145674365e6, 1.7776038695837646e6, 1.778051326399917e6, 1.7779560270597646e6, 1.7781722776841295e6, 1.7783496852550039e6, 1.7796927083375785e6, 1.7802138171466647e6, 1.7802979254438113e6, 1.7808150604726132e6, 1.7809520830676013e6, 1.780977375598419e6, 1.7810198113003082e6, 1.7810302993352856e6, 1.7810302993352856e6, 1.7810302993352856e6, 1.7810879415490094e6, 1.7811186039701037e6, 1.7811244004990973e6, 1.7811244004990973e6, 1.781136961514457e6, 1.7811731596423285e6, 1.7811731596423285e6, 1.7811764336262809e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7812510032430633e6, 1.7811833477953384e6, 1.7812969582489524e6, 1.7812401543597244e6, 1.7813986795116873e6, 1.7814555466594996e6, 1.781604014637656e6, 1.7829348856386174e6, 1.7830321629896176e6, 1.783270113644533e6, 1.7834627252728376e6, 1.7834627252728376e6, 1.7834825928033749e6, 1.7833843204656173e6, 1.7834498849398056e6, 1.783879943724016e6, 1.783879943724016e6, 1.783880119512725e6, 1.7840307567892626e6, 1.7840513986389532e6, 1.78409999733843e6, 1.78409999733843e6, 1.78409999733843e6, 1.784062981663378e6, 1.7841283797335364e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6, 1.7841896069219685e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.844825859920311e6, 1.9235915272941575e6, 1.935608287563637e6, 1.8979115987009243e6, 1.933840758946451e6, 1.8789845531296472e6, 1.9116111694456497e6, 1.9046304046312377e6, 1.8388761777448026e6, 1.9507029504076925e6, 1.912007842371927e6, 1.8603491316266274e6, 1.911512449096807e6, 1.9068306892972887e6, 1.8786376867717518e6, 1.8530738446063297e6, 1.8708981588160135e6, 1.9028567831968765e6, 1.8594821255932725e6, 1.8694843462511967e6, 1.873827421717579e6, 1.8605343074418497e6, 1.875344568169843e6, 1.8418317952183192e6, 1.8888000979647497e6, 1.8561224078642945e6, 1.8955103587515522e6, 1.8631614458324914e6, 1.837978968404686e6, 1.8611154922328917e6, 1.9542239081682079e6, 1.8805588045734179e6, 1.8557219888239787e6, 1.8428269921059315e6, 1.850845844421633e6, 1.83254139844776e6, 1.886616363411176e6, 1.8410855662393756e6, 1.8576814006288722e6, 1.860662911127335e6, 1.8639341326506375e6, 1.852390224658728e6, 1.8626987296034321e6, 1.8473568306233464e6, 1.834328069689341e6, 1.8529048303167163e6, 1.8442717294826736e6, 1.8652062938633342e6, 1.8327526467269082e6, 1.8475313361058114e6, 1.8603728767815074e6, 1.8641387663089256e6, 1.8391799076931048e6, 1.8584915858753035e6, 1.8712700899883746e6, 1.8302509734261963e6, 1.8558141303777364e6, 1.8909348833967505e6, 1.842162944141861e6, 1.86261890418146e6, 1.8276165117894602e6, 1.861449195870947e6, 1.8518744184295088e6, 1.844238417397004e6, 1.8479613220917727e6, 1.8352442704201243e6, 1.8529723730485407e6, 1.845937868160789e6, 1.856296471984645e6, 1.847858997086828e6, 1.863813230462425e6, 1.864087092431211e6, 1.8346315838444042e6, 1.8334201834917357e6, 1.8455292640550886e6, 1.8332461880096975e6, 1.833296786886916e6, 1.8350054330209251e6, 1.8298836390750762e6, 1.834703492765239e6, 1.8325504117078017e6, 1.8300917259271839e6, 1.8505476602676571e6, 1.8415812334745666e6, 1.8303942424116437e6, 1.849982827744999e6, 1.854234077550447e6, 1.8464628294920675e6, 1.8494607118540336e6, 1.8425139787234385e6, 1.8366282058778303e6, 1.8310546792004816e6, 1.8790668774499986e6, 1.82749753106292e6, 1.8459556114738751e6, 1.8512297341387477e6, 1.8491264460210348e6, 1.8290736715120855e6, 1.8325697130425917e6, 1.847321992750721e6, 1.8302417558349771e6, 1.8335897714190707e6, 1.8544756857619486e6, 1.8334519595436826e6, 1.8455111905890978e6, 1.8272097693398972e6, 1.8303105400159745e6, 1.8462041943426672e6, 1.82998834569216e6, 1.8357425089774318e6, 1.829990447038991e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6, 1.8299326086306577e6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.2170109748840332, 0.420975923538208, 0.6342620849609375, 0.8047990798950195, 1.0646209716796875, 1.299083948135376, 1.5069820880889893, 1.6981289386749268, 1.9185869693756104, 2.115488052368164, 2.288831949234009, 2.4664480686187744, 2.6828861236572266, 2.8885819911956787, 3.063749074935913, 3.319378137588501, 3.577116012573242, 3.781999111175537, 3.968364953994751, 4.1559131145477295, 4.3468780517578125, 4.534065008163452, 4.724863052368164, 4.920767068862915, 5.1437389850616455, 5.3392510414123535, 5.527233123779297, 5.718959093093872, 5.91166090965271, 6.100028991699219, 6.290349960327148, 6.487628936767578, 6.687269926071167, 6.882513046264648, 7.0839269161224365, 7.393279075622559, 7.62978196144104, 7.840954065322876, 8.043560981750488, 8.418538093566895, 8.642660140991211, 8.871655941009521, 9.075879096984863, 9.30086898803711, 9.506727933883667, 9.728641986846924, 9.940046072006226, 10.184031963348389, 10.442014932632446, 10.706485033035278, 10.970775127410889, 11.220982074737549, 11.477260112762451, 11.716701984405518, 11.942866086959839, 12.15567398071289, 12.378243923187256, 12.621211051940918, 12.917832136154175, 13.218723058700562, 13.448101043701172, 13.666880130767822, 13.910454988479614, 14.131294012069702, 14.353379964828491, 14.621593952178955, 14.852880954742432, 15.10821795463562, 15.3856840133667, 15.617962121963501, 15.88341999053955, 16.129514932632446, 16.37917995452881, 16.62642502784729, 16.858176946640015, 17.146641969680786, 17.465122938156128, 17.7086501121521, 17.93396306037903, 18.175172090530396, 18.43914294242859, 18.730040073394775, 18.9907329082489, 19.231221914291382, 19.4566490650177, 19.679126977920532, 19.96303391456604, 20.225382089614868, 20.54035997390747, 20.77877902984619, 21.006338119506836, 21.23187494277954, 21.465641021728516, 21.693392992019653, 21.96266794204712, 22.207699060440063, 22.44919204711914, 22.67416501045227, 22.901966094970703, 23.164451122283936, 23.42152690887451, 23.720487117767334, 23.97630500793457, 24.281476974487305, 24.5486159324646, 24.801804065704346, 25.041836977005005, 25.2955060005188, 25.54283308982849, 25.819926977157593, 26.09351396560669, 26.349299907684326, 26.584516048431396, 26.826401948928833, 27.068099975585938, 27.3122501373291, 27.565904140472412, 27.852817058563232, 28.099420070648193, 28.344974040985107, 28.60437512397766, 28.863584995269775, 29.12250590324402, 29.373321056365967, 29.621946096420288, 29.88619303703308, 30.1322500705719, 30.396683931350708, 30.655669927597046, 30.9059100151062, 31.151909112930298, 31.407896041870117, 31.65869402885437, 31.939549922943115, 32.20306706428528, 32.45933413505554, 32.71149706840515, 32.96174097061157, 33.218327045440674, 33.477123975753784, 33.73519206047058, 33.991634130477905, 34.2440390586853, 34.51029992103577, 34.77008509635925, 35.034661054611206, 35.30063009262085, 35.59102511405945, 35.9022741317749, 36.20774292945862, 36.4774169921875, 36.73978090286255, 37.01674509048462, 37.29898405075073, 37.56891202926636, 37.83929204940796, 38.10804200172424, 38.409656047821045, 38.70213294029236, 38.97105097770691, 39.255780935287476, 39.54319405555725, 39.82488393783569, 40.11015701293945, 40.38012909889221, 40.68098592758179, 40.989989042282104, 41.27237606048584, 41.53638291358948, 41.81235408782959, 42.09061312675476, 42.355441093444824, 42.62834906578064, 42.90382790565491, 43.170778036117554, 43.444271087646484, 43.71883702278137, 43.98798894882202, 44.28340291976929, 44.58386993408203, 44.87804698944092, 45.16054105758667, 45.440014123916626, 45.71867799758911, 45.99473810195923, 46.27721905708313, 46.56890392303467, 46.85489010810852, 47.13891291618347, 47.46004390716553, 47.74068903923035, 48.035195112228394, 48.322072982788086, 48.616661071777344, 48.908857107162476, 49.20723009109497, 49.519526958465576, 49.8065869808197, 50.13828110694885, 50.440913915634155, 50.72713899612427, 51.02223205566406, 51.326622009277344, 51.615500926971436, 51.911433935165405, 52.22265100479126, 52.51636099815369, 52.82677412033081, 53.13448405265808, 53.45270013809204, 53.749431133270264, 54.055728912353516, 54.36363410949707, 54.685028076171875, 55.02834105491638, 55.33652400970459, 55.649632930755615, 55.972492933273315, 56.32651209831238, 56.671005964279175, 56.979284048080444, 57.30537700653076, 57.6148841381073, 57.929829120635986, 58.2433340549469, 58.55705809593201, 58.901336908340454, 59.21519494056702, 59.62680912017822, 60.11589193344116, 60.433501958847046, 60.7575569152832, 61.08746600151062, 61.420356035232544, 61.73575210571289, 62.0554780960083, 62.40244197845459, 62.73930907249451, 63.06968712806702, 63.3949511051178, 63.751611948013306, 64.10331201553345, 64.42688298225403, 64.77269005775452, 65.09925103187561, 65.42950010299683, 65.76434302330017, 66.09080791473389, 66.44876503944397, 66.81897807121277, 67.23022103309631, 67.59852695465088, 67.92829203605652, 68.29792213439941, 68.6407151222229, 68.98488211631775, 69.31850099563599, 69.68238997459412, 70.04766798019409, 70.40336298942566, 70.76011610031128, 71.09925699234009, 71.44280505180359, 71.78029012680054, 72.121591091156, 72.4776771068573, 72.83292698860168, 73.19559597969055, 73.54357290267944, 73.88945603370667, 74.24208092689514, 74.58074712753296, 74.93252301216125, 75.31930494308472, 75.71694803237915, 76.07922005653381, 76.42371892929077, 76.80217099189758, 77.17865800857544, 77.54115700721741, 77.90282201766968, 78.2473349571228, 78.6165189743042, 78.97775101661682, 79.34721899032593, 79.72959613800049, 80.09367203712463, 80.44392013549805, 80.80441999435425, 81.18375301361084, 81.54305696487427, 81.91582202911377, 82.28796696662903, 82.6529541015625, 83.04258012771606, 83.41202211380005, 83.79278993606567, 84.17362594604492, 84.55813694000244, 84.92512011528015, 85.29948997497559, 85.6802110671997, 86.08356809616089, 86.51866793632507, 86.92366909980774, 87.32803797721863, 87.69828391075134, 88.12548398971558, 88.50426912307739, 88.88273501396179, 89.31951808929443, 89.69777297973633, 90.07481098175049, 90.4558961391449, 90.82615900039673, 91.2084550857544, 91.59082508087158, 91.99743103981018, 92.40339493751526, 92.81288695335388, 93.20149397850037, 93.58510899543762, 93.97773313522339, 94.37523603439331, 94.7634711265564, 95.18019700050354, 95.58136892318726, 95.99146294593811, 96.38400197029114, 96.78503608703613, 97.18385791778564, 97.59602904319763, 97.98753213882446, 98.38272500038147, 98.779541015625, 99.197340965271, 99.58721804618835, 99.9836790561676, 100.39483213424683, 100.79816794395447, 101.19381713867188, 101.62127113342285, 102.04188799858093, 102.45606708526611, 102.85920190811157, 103.27209711074829, 103.68746399879456, 104.10347700119019, 104.50968098640442, 104.92449808120728, 105.34757995605469, 105.77484011650085, 106.18914103507996, 106.6019959449768, 107.0039119720459, 107.43312907218933, 107.87829303741455, 108.28986597061157, 108.7134599685669, 109.14668297767639, 109.57151913642883, 109.98572111129761, 110.4020459651947, 110.82567000389099, 111.24483609199524, 111.69871091842651, 112.12747502326965, 112.58052897453308, 113.00352907180786, 113.4379870891571, 113.8611650466919, 114.29394912719727, 114.7146589756012, 115.16397905349731, 115.59817910194397, 116.062264919281, 116.48990392684937, 116.92436504364014, 117.35360193252563, 117.80435299873352, 118.25913310050964, 118.71456503868103, 119.15598893165588, 119.59567093849182, 120.03145003318787, 120.47516798973083, 120.9235200881958, 121.37053394317627, 121.82250499725342, 122.26094698905945, 122.71715998649597, 123.18779802322388, 123.64577293395996, 124.11889910697937, 124.56356501579285, 125.0460000038147, 125.48903703689575, 125.93962812423706, 126.42126107215881, 126.87419295310974, 127.34009909629822, 127.78910899162292, 128.249342918396, 128.72653198242188, 129.18513703346252, 129.6587209701538, 130.1221420764923, 130.60781002044678, 131.0533230304718, 131.52389407157898, 132.00872707366943, 132.47075200080872, 132.9452259540558, 133.40594506263733, 133.8964340686798, 134.36643505096436, 134.83475303649902, 135.3274531364441, 135.82721304893494, 136.33352613449097, 136.8003580570221, 137.30535292625427, 137.77178597450256, 138.24804091453552, 138.76191091537476, 139.23580193519592, 139.73629808425903, 140.2075400352478, 140.71346998214722, 141.1903591156006, 141.68032312393188, 142.1675329208374, 142.6471071243286, 143.15776801109314, 143.64264798164368, 144.15607810020447, 144.73192310333252, 145.39513611793518, 145.87700700759888, 146.38958597183228, 146.8883559703827, 147.4103410243988, 147.9343650341034, 148.46503591537476, 148.94963312149048, 149.4417769908905, 149.95818710327148, 150.44953513145447, 150.9694631099701, 151.4705901145935, 151.99269604682922, 152.4839689731598, 153.0140299797058, 153.5068039894104, 154.03389406204224, 154.52637195587158, 155.02848100662231, 155.55282402038574, 156.06574392318726, 156.59384894371033, 157.0967309474945, 157.63075804710388, 158.13560509681702, 158.65127301216125, 159.15374994277954, 159.6987681388855, 160.20227313041687, 160.75287199020386, 161.25744605064392, 161.76950001716614, 162.3123641014099, 162.82893800735474, 163.3703260421753, 163.88657593727112, 164.43132400512695, 164.9469199180603, 165.48073506355286, 166.01245713233948, 166.5433111190796, 167.06061911582947, 167.6156120300293, 168.13484001159668, 168.68810510635376, 169.20773696899414, 169.75022411346436, 170.27359414100647, 170.83176612854004, 171.36738991737366, 171.92639112472534, 172.46731400489807, 173.00261211395264, 173.56184601783752, 174.09663105010986, 174.65756797790527, 175.1914529800415, 175.78752493858337, 176.32831597328186, 176.89525294303894, 177.4769570827484, 178.07331490516663, 178.63575792312622, 179.20663905143738, 179.74860000610352, 180.3252100944519, 180.87682008743286, 181.46176195144653, 182.0100519657135, 182.57846593856812, 183.12716913223267, 183.72383904457092, 184.27356100082397, 184.84884691238403, 185.39460110664368, 185.9788579940796, 186.53601503372192, 187.12522292137146, 187.67679500579834, 188.2669939994812, 188.81868195533752, 189.40350008010864, 189.96092200279236, 190.55601501464844, 191.36281490325928, 191.9448220729828, 192.5365080833435, 193.11559295654297, 193.6858811378479, 194.28021097183228, 194.842768907547, 195.44774198532104, 196.0452160835266, 196.65674996376038, 197.2472620010376, 197.83662796020508, 198.43131613731384, 199.0087649822235, 199.62626600265503, 200.20629501342773, 200.8223581314087, 201.39200711250305, 202.0026240348816, 202.58548402786255, 203.20348000526428, 203.7865331172943, 204.41680598258972, 205.00267696380615, 205.61913013458252, 206.20760011672974, 206.82732701301575, 207.41450095176697, 208.06042194366455, 208.6627209186554, 209.26020407676697, 209.84974193572998, 210.46118903160095, 211.08398699760437, 211.71374702453613, 212.33252596855164, 212.92987608909607, 213.555762052536, 214.15740394592285, 214.7888400554657, 215.3837571144104, 216.0020251274109, 216.60126113891602, 217.2445559501648, 217.8483989238739, 218.48076605796814, 219.08856010437012, 219.7833490371704, 220.58951902389526, 221.19135808944702, 221.8606879711151, 222.4738209247589, 223.10128211975098, 223.7075400352478, 224.3427951335907, 224.95079803466797, 225.5931360721588, 226.2183449268341, 226.84245705604553, 227.50377011299133, 228.1145830154419, 228.76066613197327, 229.38882899284363, 230.03243112564087, 230.6485230922699, 231.30374693870544, 231.92868900299072, 232.59324598312378, 233.24675297737122, 233.8831820487976, 234.53902506828308, 235.16483306884766, 235.83566999435425, 236.46190404891968, 237.1135709285736, 237.7613229751587, 238.41159105300903, 239.08026313781738, 239.7209551334381, 240.3947880268097, 241.0341739654541, 241.69950890541077, 242.36247992515564, 243.07301998138428, 243.89843201637268, 244.55713605880737, 245.24813890457153, 245.932932138443, 246.59419798851013, 247.2743821144104, 247.92984890937805, 248.6165680885315, 249.2810320854187, 249.9528341293335, 250.63934898376465, 251.30342602729797, 251.95526790618896, 252.60899090766907, 253.30463194847107, 253.97177696228027, 254.66177797317505, 255.3405420780182, 255.99825596809387, 256.69389605522156, 257.3656361103058, 258.0513050556183, 258.75511407852173, 259.4350709915161, 260.12226700782776, 260.78859996795654, 261.50559997558594, 262.20134711265564, 262.8661150932312, 263.6461660861969, 264.5113580226898, 265.1795630455017, 265.91611194610596, 266.5990159511566, 267.31254601478577, 268.0374550819397, 268.7464120388031, 269.4658989906311, 270.1434509754181, 270.85572600364685, 271.5723171234131, 272.2650730609894, 272.9831690788269, 273.6944329738617, 274.4147629737854, 275.13687205314636, 275.82865810394287, 276.5430200099945, 277.2239451408386, 277.95701003074646, 278.672621011734, 279.3702619075775, 280.1015341281891, 280.9238269329071, 281.6211619377136, 282.36277294158936, 283.1026051044464, 283.9950981140137, 284.7471590042114, 285.46673107147217, 286.1952350139618, 286.9365859031677, 287.64865708351135, 288.3865830898285, 289.10041093826294, 289.8395130634308, 290.58754801750183, 291.30743312835693, 292.0533230304718, 292.7883999347687, 293.52814412117004, 294.2861111164093, 295.0027461051941, 295.7454330921173, 296.4790050983429, 297.2337050437927, 297.9737250804901, 298.72052812576294, 299.4729459285736, 300.20584511756897, 300.9563419818878, 301.9289231300354, 302.6547191143036, 303.42950797080994, 304.1989040374756, 304.9559819698334, 305.7123920917511, 306.45812702178955, 307.2076361179352, 307.9912860393524, 308.7275059223175, 309.49905610084534, 310.27139711380005, 311.01569390296936, 311.76397490501404, 312.5484199523926, 313.294734954834, 314.07049107551575, 314.8217439651489, 315.58386492729187, 316.37455010414124, 317.12751293182373, 317.911602973938, 318.76011300086975, 319.66675996780396, 320.46563506126404, 321.2479500770569, 322.00206899642944, 322.7928841114044, 323.578537940979, 324.3474600315094, 325.133661031723, 325.93194699287415, 326.6849961280823, 327.47613310813904, 328.2640359401703, 329.03504610061646, 329.8227369785309, 330.6332230567932, 331.4032371044159, 332.2083549499512, 333.02950406074524, 333.82567596435547, 334.62665605545044, 335.47402691841125, 336.4039249420166, 337.23444509506226, 338.08509492874146, 338.8700520992279, 339.6784551143646, 340.5246241092682, 341.3263261318207, 342.1294310092926, 342.9909620285034, 343.76706099510193, 344.5852599143982, 345.4187180995941, 346.218150138855, 347.0424699783325, 347.858029127121, 348.69944405555725, 349.4972081184387, 350.3276469707489, 351.15716791152954, 351.9937069416046, 353.0152130126953, 353.8746781349182, 354.7010350227356, 355.51815605163574, 356.35655093193054, 357.18858909606934, 358.0019631385803, 358.8308970928192, 359.6735429763794, 360.4920799732208, 361.3214259147644, 362.16600799560547, 362.9728569984436, 363.8163471221924, 364.6769869327545, 365.5122821331024, 366.360426902771, 367.20548701286316, 368.0492980480194, 368.93330001831055, 369.92498111724854, 370.80468106269836, 371.62778902053833, 372.49510192871094, 373.3600869178772, 374.2265191078186, 375.0551459789276, 375.92515897750854, 376.8139021396637, 377.64042592048645, 378.5063660144806, 379.36422204971313, 380.201287984848, 381.0786199569702, 381.94054794311523, 382.82108902931213, 383.6605079174042, 384.5340840816498, 385.40913105010986, 386.48436307907104, 387.39362692832947, 388.2735059261322, 389.166944026947, 390.0230929851532, 390.9127631187439, 391.8083760738373, 392.65189003944397, 393.5502059459686, 394.4399049282074, 395.3048930168152, 396.187618970871, 397.0909249782562, 397.9602270126343, 398.8432400226593, 399.7191319465637, 400.63164806365967, 401.53097701072693, 402.4824409484863, 403.53404903411865, 404.45128297805786, 405.3215250968933, 406.22948694229126, 407.17128109931946, 408.0381979942322, 408.9460771083832, 409.8477430343628, 410.74157094955444, 411.61957597732544, 412.5260260105133, 413.4705069065094, 414.3971481323242, 415.28069400787354, 416.17723393440247, 417.10404896736145, 418.0425500869751, 419.1466660499573, 420.0810251235962, 421.0043671131134, 421.89977407455444, 422.809180021286, 423.7377669811249, 424.67258501052856, 425.5745370388031, 426.5110321044922, 427.44792103767395, 428.3676481246948, 429.273579120636, 430.20401191711426, 431.1469750404358, 432.0421290397644, 432.98137307167053, 433.96869707107544, 435.05565190315247, 436.0112750530243, 436.9404299259186, 437.88771200180054, 438.8279480934143, 439.73924493789673, 440.6741781234741, 441.60400009155273, 442.5551669597626, 443.4806020259857, 444.43926906585693, 445.3844051361084, 446.35151290893555, 447.2791340351105, 448.23642897605896, 449.20076608657837, 450.241534948349, 451.35938906669617, 452.3399851322174, 453.31347703933716, 454.29880690574646, 455.2388949394226, 456.1987130641937, 457.1720941066742, 458.1779580116272, 459.1200840473175, 460.0917420387268, 461.0532240867615, 462.0427529811859, 462.98223900794983, 463.93627190589905, 464.9021461009979, 465.92756700515747, 467.032310962677, 468.02534198760986, 469.04761600494385, 470.03959012031555, 471.01448798179626, 471.9883029460907, 473.00123596191406, 473.99528312683105, 474.9555289745331, 475.94361901283264, 476.93494606018066, 477.9338390827179, 478.9212019443512, 479.9446461200714, 480.9696989059448, 482.1220610141754, 483.13476395606995, 484.0949709415436, 485.10562205314636, 486.11592292785645, 487.1251001358032, 488.1008129119873, 489.1332459449768, 490.13913202285767, 491.14870595932007, 492.1494970321655, 493.12780594825745, 494.1282820701599, 495.1263520717621, 496.1918680667877, 497.3599500656128, 498.35625290870667, 499.4162509441376, 500.4233160018921, 501.4461989402771, 502.4473810195923, 503.4579920768738, 504.48466992378235, 505.49614095687866, 506.5291950702667, 507.5274510383606, 508.5595290660858, 509.61520290374756, 510.6342489719391, 511.7157530784607, 512.9154751300812, 513.9610970020294, 515.0167319774628, 516.0746309757233, 517.0741839408875, 518.1237449645996, 519.1894330978394, 520.2691569328308, 521.2849459648132, 522.3174540996552, 523.3594279289246, 524.405534029007, 525.4520189762115, 526.4731600284576, 527.7196531295776, 528.7606179714203, 529.8835020065308, 530.9367680549622, 531.9845960140228, 533.0273489952087, 534.0878989696503, 535.158280134201, 536.2233049869537, 537.2367029190063, 538.3021919727325, 539.3924031257629, 540.4600629806519, 541.5288689136505, 542.8045699596405, 543.8606679439545, 544.9393999576569, 546.0143630504608, 547.0892550945282, 548.2317500114441, 549.2812640666962, 550.3729989528656, 551.458734035492, 552.5419471263885, 553.6251881122589, 554.6768579483032, 555.7637920379639, 556.9027800559998, 558.1529150009155, 559.2652819156647, 560.3734319210052, 561.443165063858, 562.5486240386963, 563.6399729251862, 564.7375259399414, 565.8284430503845, 566.8974311351776, 567.9951810836792, 569.0811560153961, 570.1928551197052, 571.2926790714264, 572.4569230079651, 573.6804001331329, 574.8125910758972, 575.9124090671539, 577.0288379192352, 578.1393129825592, 579.2763910293579, 580.3766329288483, 581.4946939945221, 582.6100370883942, 583.720330953598, 584.8477640151978, 585.9366600513458, 587.0663440227509, 588.3887629508972, 589.5698680877686, 590.7203750610352, 591.8552989959717, 592.9535441398621, 594.1034119129181, 595.2432360649109, 596.3796761035919, 597.5080800056458, 598.6126251220703]</t>
   </si>
 </sst>
 </file>
@@ -77,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -99,12 +111,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,12 +155,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,9 +184,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.04"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -200,8 +199,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -210,50 +209,50 @@
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1082.28656005859</v>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>2408.456635952</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1674.21192502975</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>583.807985067368</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>